<commit_message>
[DOC] Schedule update - Trans PCB 입고
</commit_message>
<xml_diff>
--- a/0_DOC/Femto Project schedule V1.0.xlsx
+++ b/0_DOC/Femto Project schedule V1.0.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390"/>
@@ -12,12 +12,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'20180207'!$A$1:$EH$49</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
   <si>
     <t>◇PCB설계</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -190,6 +190,10 @@
     <t>◇ 회로도 입수</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>◇PCB 입고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -937,6 +941,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -970,26 +994,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1125,8 +1129,8 @@
       <xdr:rowOff>80806</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>45</xdr:col>
-      <xdr:colOff>157370</xdr:colOff>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>80806</xdr:rowOff>
     </xdr:to>
@@ -1137,8 +1141,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9315451" y="3493241"/>
-          <a:ext cx="847310" cy="0"/>
+          <a:off x="9134890" y="3976531"/>
+          <a:ext cx="685385" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2215,7 +2219,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2250,7 +2254,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2461,9 +2465,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EV66"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BX46" sqref="BX46"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BB27" sqref="BB27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2499,167 +2503,167 @@
     </row>
     <row r="6" spans="1:152" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="113">
+      <c r="B6" s="129">
         <v>1</v>
       </c>
-      <c r="C6" s="110"/>
-      <c r="D6" s="110"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="110"/>
-      <c r="I6" s="110"/>
-      <c r="J6" s="110"/>
-      <c r="K6" s="110"/>
-      <c r="L6" s="110"/>
-      <c r="M6" s="110"/>
-      <c r="N6" s="110"/>
-      <c r="O6" s="110"/>
-      <c r="P6" s="110"/>
-      <c r="Q6" s="110"/>
-      <c r="R6" s="110"/>
-      <c r="S6" s="110"/>
-      <c r="T6" s="110"/>
-      <c r="U6" s="110"/>
-      <c r="V6" s="110"/>
-      <c r="W6" s="110"/>
-      <c r="X6" s="110"/>
-      <c r="Y6" s="110"/>
-      <c r="Z6" s="110"/>
-      <c r="AA6" s="110"/>
-      <c r="AB6" s="110"/>
-      <c r="AC6" s="110"/>
-      <c r="AD6" s="110"/>
-      <c r="AE6" s="110"/>
-      <c r="AF6" s="110"/>
-      <c r="AG6" s="113">
+      <c r="C6" s="126"/>
+      <c r="D6" s="126"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="126"/>
+      <c r="G6" s="126"/>
+      <c r="H6" s="126"/>
+      <c r="I6" s="126"/>
+      <c r="J6" s="126"/>
+      <c r="K6" s="126"/>
+      <c r="L6" s="126"/>
+      <c r="M6" s="126"/>
+      <c r="N6" s="126"/>
+      <c r="O6" s="126"/>
+      <c r="P6" s="126"/>
+      <c r="Q6" s="126"/>
+      <c r="R6" s="126"/>
+      <c r="S6" s="126"/>
+      <c r="T6" s="126"/>
+      <c r="U6" s="126"/>
+      <c r="V6" s="126"/>
+      <c r="W6" s="126"/>
+      <c r="X6" s="126"/>
+      <c r="Y6" s="126"/>
+      <c r="Z6" s="126"/>
+      <c r="AA6" s="126"/>
+      <c r="AB6" s="126"/>
+      <c r="AC6" s="126"/>
+      <c r="AD6" s="126"/>
+      <c r="AE6" s="126"/>
+      <c r="AF6" s="126"/>
+      <c r="AG6" s="129">
         <v>2</v>
       </c>
-      <c r="AH6" s="110"/>
-      <c r="AI6" s="110"/>
-      <c r="AJ6" s="110"/>
-      <c r="AK6" s="110"/>
-      <c r="AL6" s="110"/>
-      <c r="AM6" s="110"/>
-      <c r="AN6" s="110"/>
-      <c r="AO6" s="110"/>
-      <c r="AP6" s="110"/>
-      <c r="AQ6" s="110"/>
-      <c r="AR6" s="110"/>
-      <c r="AS6" s="110"/>
-      <c r="AT6" s="110"/>
-      <c r="AU6" s="110"/>
-      <c r="AV6" s="110"/>
-      <c r="AW6" s="110"/>
-      <c r="AX6" s="110"/>
-      <c r="AY6" s="110"/>
-      <c r="AZ6" s="110"/>
-      <c r="BA6" s="110"/>
-      <c r="BB6" s="110"/>
-      <c r="BC6" s="110"/>
-      <c r="BD6" s="110"/>
-      <c r="BE6" s="110"/>
-      <c r="BF6" s="110"/>
-      <c r="BG6" s="110"/>
-      <c r="BH6" s="111"/>
-      <c r="BI6" s="110">
+      <c r="AH6" s="126"/>
+      <c r="AI6" s="126"/>
+      <c r="AJ6" s="126"/>
+      <c r="AK6" s="126"/>
+      <c r="AL6" s="126"/>
+      <c r="AM6" s="126"/>
+      <c r="AN6" s="126"/>
+      <c r="AO6" s="126"/>
+      <c r="AP6" s="126"/>
+      <c r="AQ6" s="126"/>
+      <c r="AR6" s="126"/>
+      <c r="AS6" s="126"/>
+      <c r="AT6" s="126"/>
+      <c r="AU6" s="126"/>
+      <c r="AV6" s="126"/>
+      <c r="AW6" s="126"/>
+      <c r="AX6" s="126"/>
+      <c r="AY6" s="126"/>
+      <c r="AZ6" s="126"/>
+      <c r="BA6" s="126"/>
+      <c r="BB6" s="126"/>
+      <c r="BC6" s="126"/>
+      <c r="BD6" s="126"/>
+      <c r="BE6" s="126"/>
+      <c r="BF6" s="126"/>
+      <c r="BG6" s="126"/>
+      <c r="BH6" s="127"/>
+      <c r="BI6" s="126">
         <v>3</v>
       </c>
-      <c r="BJ6" s="110"/>
-      <c r="BK6" s="110"/>
-      <c r="BL6" s="110"/>
-      <c r="BM6" s="110"/>
-      <c r="BN6" s="110"/>
-      <c r="BO6" s="110"/>
-      <c r="BP6" s="110"/>
-      <c r="BQ6" s="110"/>
-      <c r="BR6" s="110"/>
-      <c r="BS6" s="110"/>
-      <c r="BT6" s="110"/>
-      <c r="BU6" s="110"/>
-      <c r="BV6" s="110"/>
-      <c r="BW6" s="110"/>
-      <c r="BX6" s="110"/>
-      <c r="BY6" s="110"/>
-      <c r="BZ6" s="110"/>
-      <c r="CA6" s="110"/>
-      <c r="CB6" s="110"/>
-      <c r="CC6" s="110"/>
-      <c r="CD6" s="110"/>
-      <c r="CE6" s="110"/>
-      <c r="CF6" s="110"/>
-      <c r="CG6" s="110"/>
-      <c r="CH6" s="110"/>
-      <c r="CI6" s="110"/>
-      <c r="CJ6" s="110"/>
-      <c r="CK6" s="110"/>
-      <c r="CL6" s="110"/>
-      <c r="CM6" s="110"/>
-      <c r="CN6" s="114">
+      <c r="BJ6" s="126"/>
+      <c r="BK6" s="126"/>
+      <c r="BL6" s="126"/>
+      <c r="BM6" s="126"/>
+      <c r="BN6" s="126"/>
+      <c r="BO6" s="126"/>
+      <c r="BP6" s="126"/>
+      <c r="BQ6" s="126"/>
+      <c r="BR6" s="126"/>
+      <c r="BS6" s="126"/>
+      <c r="BT6" s="126"/>
+      <c r="BU6" s="126"/>
+      <c r="BV6" s="126"/>
+      <c r="BW6" s="126"/>
+      <c r="BX6" s="126"/>
+      <c r="BY6" s="126"/>
+      <c r="BZ6" s="126"/>
+      <c r="CA6" s="126"/>
+      <c r="CB6" s="126"/>
+      <c r="CC6" s="126"/>
+      <c r="CD6" s="126"/>
+      <c r="CE6" s="126"/>
+      <c r="CF6" s="126"/>
+      <c r="CG6" s="126"/>
+      <c r="CH6" s="126"/>
+      <c r="CI6" s="126"/>
+      <c r="CJ6" s="126"/>
+      <c r="CK6" s="126"/>
+      <c r="CL6" s="126"/>
+      <c r="CM6" s="126"/>
+      <c r="CN6" s="130">
         <v>4</v>
       </c>
-      <c r="CO6" s="115"/>
-      <c r="CP6" s="115"/>
-      <c r="CQ6" s="115"/>
-      <c r="CR6" s="115"/>
-      <c r="CS6" s="115"/>
-      <c r="CT6" s="115"/>
-      <c r="CU6" s="115"/>
-      <c r="CV6" s="115"/>
-      <c r="CW6" s="115"/>
-      <c r="CX6" s="115"/>
-      <c r="CY6" s="115"/>
-      <c r="CZ6" s="115"/>
-      <c r="DA6" s="115"/>
-      <c r="DB6" s="115"/>
-      <c r="DC6" s="115"/>
-      <c r="DD6" s="115"/>
-      <c r="DE6" s="115"/>
-      <c r="DF6" s="115"/>
-      <c r="DG6" s="115"/>
-      <c r="DH6" s="115"/>
-      <c r="DI6" s="115"/>
-      <c r="DJ6" s="115"/>
-      <c r="DK6" s="115"/>
-      <c r="DL6" s="115"/>
-      <c r="DM6" s="115"/>
-      <c r="DN6" s="115"/>
-      <c r="DO6" s="115"/>
-      <c r="DP6" s="115"/>
-      <c r="DQ6" s="116"/>
-      <c r="DR6" s="110">
+      <c r="CO6" s="131"/>
+      <c r="CP6" s="131"/>
+      <c r="CQ6" s="131"/>
+      <c r="CR6" s="131"/>
+      <c r="CS6" s="131"/>
+      <c r="CT6" s="131"/>
+      <c r="CU6" s="131"/>
+      <c r="CV6" s="131"/>
+      <c r="CW6" s="131"/>
+      <c r="CX6" s="131"/>
+      <c r="CY6" s="131"/>
+      <c r="CZ6" s="131"/>
+      <c r="DA6" s="131"/>
+      <c r="DB6" s="131"/>
+      <c r="DC6" s="131"/>
+      <c r="DD6" s="131"/>
+      <c r="DE6" s="131"/>
+      <c r="DF6" s="131"/>
+      <c r="DG6" s="131"/>
+      <c r="DH6" s="131"/>
+      <c r="DI6" s="131"/>
+      <c r="DJ6" s="131"/>
+      <c r="DK6" s="131"/>
+      <c r="DL6" s="131"/>
+      <c r="DM6" s="131"/>
+      <c r="DN6" s="131"/>
+      <c r="DO6" s="131"/>
+      <c r="DP6" s="131"/>
+      <c r="DQ6" s="132"/>
+      <c r="DR6" s="126">
         <v>5</v>
       </c>
-      <c r="DS6" s="110"/>
-      <c r="DT6" s="110"/>
-      <c r="DU6" s="110"/>
-      <c r="DV6" s="110"/>
-      <c r="DW6" s="110"/>
-      <c r="DX6" s="110"/>
-      <c r="DY6" s="110"/>
-      <c r="DZ6" s="110"/>
-      <c r="EA6" s="110"/>
-      <c r="EB6" s="110"/>
-      <c r="EC6" s="110"/>
-      <c r="ED6" s="110"/>
-      <c r="EE6" s="110"/>
-      <c r="EF6" s="110"/>
-      <c r="EG6" s="110"/>
-      <c r="EH6" s="110"/>
-      <c r="EI6" s="110"/>
-      <c r="EJ6" s="110"/>
-      <c r="EK6" s="110"/>
-      <c r="EL6" s="110"/>
-      <c r="EM6" s="110"/>
-      <c r="EN6" s="110"/>
-      <c r="EO6" s="110"/>
-      <c r="EP6" s="110"/>
-      <c r="EQ6" s="110"/>
-      <c r="ER6" s="110"/>
-      <c r="ES6" s="110"/>
-      <c r="ET6" s="110"/>
-      <c r="EU6" s="110"/>
-      <c r="EV6" s="111"/>
+      <c r="DS6" s="126"/>
+      <c r="DT6" s="126"/>
+      <c r="DU6" s="126"/>
+      <c r="DV6" s="126"/>
+      <c r="DW6" s="126"/>
+      <c r="DX6" s="126"/>
+      <c r="DY6" s="126"/>
+      <c r="DZ6" s="126"/>
+      <c r="EA6" s="126"/>
+      <c r="EB6" s="126"/>
+      <c r="EC6" s="126"/>
+      <c r="ED6" s="126"/>
+      <c r="EE6" s="126"/>
+      <c r="EF6" s="126"/>
+      <c r="EG6" s="126"/>
+      <c r="EH6" s="126"/>
+      <c r="EI6" s="126"/>
+      <c r="EJ6" s="126"/>
+      <c r="EK6" s="126"/>
+      <c r="EL6" s="126"/>
+      <c r="EM6" s="126"/>
+      <c r="EN6" s="126"/>
+      <c r="EO6" s="126"/>
+      <c r="EP6" s="126"/>
+      <c r="EQ6" s="126"/>
+      <c r="ER6" s="126"/>
+      <c r="ES6" s="126"/>
+      <c r="ET6" s="126"/>
+      <c r="EU6" s="126"/>
+      <c r="EV6" s="127"/>
     </row>
     <row r="7" spans="1:152" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
@@ -2849,19 +2853,19 @@
       <c r="BK7" s="10">
         <v>3</v>
       </c>
-      <c r="BL7" s="117">
+      <c r="BL7" s="106">
         <v>4</v>
       </c>
-      <c r="BM7" s="118">
+      <c r="BM7" s="107">
         <v>5</v>
       </c>
-      <c r="BN7" s="118">
+      <c r="BN7" s="107">
         <v>6</v>
       </c>
-      <c r="BO7" s="118">
+      <c r="BO7" s="107">
         <v>7</v>
       </c>
-      <c r="BP7" s="118">
+      <c r="BP7" s="107">
         <v>8</v>
       </c>
       <c r="BQ7" s="8">
@@ -3118,7 +3122,7 @@
       </c>
     </row>
     <row r="8" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A8" s="107" t="s">
+      <c r="A8" s="123" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="34"/>
@@ -3189,11 +3193,11 @@
       <c r="BI8" s="38"/>
       <c r="BJ8" s="35"/>
       <c r="BK8" s="38"/>
-      <c r="BL8" s="119"/>
-      <c r="BM8" s="120"/>
-      <c r="BN8" s="119"/>
-      <c r="BO8" s="121"/>
-      <c r="BP8" s="119"/>
+      <c r="BL8" s="108"/>
+      <c r="BM8" s="109"/>
+      <c r="BN8" s="108"/>
+      <c r="BO8" s="110"/>
+      <c r="BP8" s="108"/>
       <c r="BQ8" s="35"/>
       <c r="BR8" s="38"/>
       <c r="BS8" s="38"/>
@@ -3280,7 +3284,7 @@
       <c r="EV8" s="100"/>
     </row>
     <row r="9" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A9" s="107"/>
+      <c r="A9" s="123"/>
       <c r="B9" s="29"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
@@ -3347,11 +3351,11 @@
       <c r="BI9" s="31"/>
       <c r="BJ9" s="30"/>
       <c r="BK9" s="31"/>
-      <c r="BL9" s="122"/>
-      <c r="BM9" s="122"/>
-      <c r="BN9" s="122"/>
-      <c r="BO9" s="122"/>
-      <c r="BP9" s="122"/>
+      <c r="BL9" s="111"/>
+      <c r="BM9" s="111"/>
+      <c r="BN9" s="111"/>
+      <c r="BO9" s="111"/>
+      <c r="BP9" s="111"/>
       <c r="BQ9" s="30"/>
       <c r="BR9" s="31"/>
       <c r="BS9" s="31"/>
@@ -3438,7 +3442,7 @@
       <c r="EV9" s="33"/>
     </row>
     <row r="10" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A10" s="107"/>
+      <c r="A10" s="123"/>
       <c r="B10" s="29"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
@@ -3505,11 +3509,11 @@
       <c r="BI10" s="31"/>
       <c r="BJ10" s="30"/>
       <c r="BK10" s="31"/>
-      <c r="BL10" s="122"/>
-      <c r="BM10" s="122"/>
-      <c r="BN10" s="122"/>
-      <c r="BO10" s="122"/>
-      <c r="BP10" s="122"/>
+      <c r="BL10" s="111"/>
+      <c r="BM10" s="111"/>
+      <c r="BN10" s="111"/>
+      <c r="BO10" s="111"/>
+      <c r="BP10" s="111"/>
       <c r="BQ10" s="30"/>
       <c r="BR10" s="31"/>
       <c r="BS10" s="31"/>
@@ -3596,7 +3600,7 @@
       <c r="EV10" s="33"/>
     </row>
     <row r="11" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A11" s="107"/>
+      <c r="A11" s="123"/>
       <c r="B11" s="29"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
@@ -3663,11 +3667,11 @@
       <c r="BI11" s="31"/>
       <c r="BJ11" s="30"/>
       <c r="BK11" s="31"/>
-      <c r="BL11" s="122"/>
-      <c r="BM11" s="122"/>
-      <c r="BN11" s="122"/>
-      <c r="BO11" s="122"/>
-      <c r="BP11" s="122"/>
+      <c r="BL11" s="111"/>
+      <c r="BM11" s="111"/>
+      <c r="BN11" s="111"/>
+      <c r="BO11" s="111"/>
+      <c r="BP11" s="111"/>
       <c r="BQ11" s="30"/>
       <c r="BR11" s="31"/>
       <c r="BS11" s="31"/>
@@ -3754,7 +3758,7 @@
       <c r="EV11" s="33"/>
     </row>
     <row r="12" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A12" s="107"/>
+      <c r="A12" s="123"/>
       <c r="B12" s="29"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
@@ -3821,11 +3825,11 @@
       <c r="BI12" s="31"/>
       <c r="BJ12" s="30"/>
       <c r="BK12" s="31"/>
-      <c r="BL12" s="122"/>
-      <c r="BM12" s="122"/>
-      <c r="BN12" s="122"/>
-      <c r="BO12" s="122"/>
-      <c r="BP12" s="122"/>
+      <c r="BL12" s="111"/>
+      <c r="BM12" s="111"/>
+      <c r="BN12" s="111"/>
+      <c r="BO12" s="111"/>
+      <c r="BP12" s="111"/>
       <c r="BQ12" s="30"/>
       <c r="BR12" s="31"/>
       <c r="BS12" s="31"/>
@@ -3912,7 +3916,7 @@
       <c r="EV12" s="33"/>
     </row>
     <row r="13" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A13" s="107"/>
+      <c r="A13" s="123"/>
       <c r="B13" s="29"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -3977,11 +3981,11 @@
       <c r="BI13" s="31"/>
       <c r="BJ13" s="30"/>
       <c r="BK13" s="31"/>
-      <c r="BL13" s="122"/>
-      <c r="BM13" s="122"/>
-      <c r="BN13" s="122"/>
-      <c r="BO13" s="122"/>
-      <c r="BP13" s="122"/>
+      <c r="BL13" s="111"/>
+      <c r="BM13" s="111"/>
+      <c r="BN13" s="111"/>
+      <c r="BO13" s="111"/>
+      <c r="BP13" s="111"/>
       <c r="BQ13" s="30"/>
       <c r="BR13" s="31"/>
       <c r="BS13" s="31"/>
@@ -4068,7 +4072,7 @@
       <c r="EV13" s="33"/>
     </row>
     <row r="14" spans="1:152" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="112"/>
+      <c r="A14" s="128"/>
       <c r="B14" s="51"/>
       <c r="C14" s="52"/>
       <c r="D14" s="52"/>
@@ -4131,11 +4135,11 @@
       <c r="BI14" s="53"/>
       <c r="BJ14" s="52"/>
       <c r="BK14" s="53"/>
-      <c r="BL14" s="123"/>
-      <c r="BM14" s="123"/>
-      <c r="BN14" s="123"/>
-      <c r="BO14" s="123"/>
-      <c r="BP14" s="123"/>
+      <c r="BL14" s="112"/>
+      <c r="BM14" s="112"/>
+      <c r="BN14" s="112"/>
+      <c r="BO14" s="112"/>
+      <c r="BP14" s="112"/>
       <c r="BQ14" s="52"/>
       <c r="BR14" s="53"/>
       <c r="BS14" s="53"/>
@@ -4222,7 +4226,7 @@
       <c r="EV14" s="101"/>
     </row>
     <row r="15" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A15" s="109" t="s">
+      <c r="A15" s="125" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="43"/>
@@ -4289,11 +4293,11 @@
       <c r="BI15" s="45"/>
       <c r="BJ15" s="47"/>
       <c r="BK15" s="45"/>
-      <c r="BL15" s="124"/>
-      <c r="BM15" s="124"/>
-      <c r="BN15" s="124"/>
-      <c r="BO15" s="124"/>
-      <c r="BP15" s="124"/>
+      <c r="BL15" s="113"/>
+      <c r="BM15" s="113"/>
+      <c r="BN15" s="113"/>
+      <c r="BO15" s="113"/>
+      <c r="BP15" s="113"/>
       <c r="BQ15" s="47" t="s">
         <v>9</v>
       </c>
@@ -4384,7 +4388,7 @@
       <c r="EV15" s="103"/>
     </row>
     <row r="16" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A16" s="107"/>
+      <c r="A16" s="123"/>
       <c r="B16" s="24"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -4449,11 +4453,11 @@
       <c r="BI16" s="14"/>
       <c r="BJ16" s="16"/>
       <c r="BK16" s="14"/>
-      <c r="BL16" s="125"/>
-      <c r="BM16" s="125"/>
-      <c r="BN16" s="125"/>
-      <c r="BO16" s="125"/>
-      <c r="BP16" s="125"/>
+      <c r="BL16" s="114"/>
+      <c r="BM16" s="114"/>
+      <c r="BN16" s="114"/>
+      <c r="BO16" s="114"/>
+      <c r="BP16" s="114"/>
       <c r="BQ16" s="16" t="s">
         <v>0</v>
       </c>
@@ -4542,7 +4546,7 @@
       <c r="EV16" s="17"/>
     </row>
     <row r="17" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A17" s="107"/>
+      <c r="A17" s="123"/>
       <c r="B17" s="24"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -4605,11 +4609,11 @@
       <c r="BI17" s="14"/>
       <c r="BJ17" s="16"/>
       <c r="BK17" s="14"/>
-      <c r="BL17" s="125"/>
-      <c r="BM17" s="125"/>
-      <c r="BN17" s="125"/>
-      <c r="BO17" s="125"/>
-      <c r="BP17" s="125"/>
+      <c r="BL17" s="114"/>
+      <c r="BM17" s="114"/>
+      <c r="BN17" s="114"/>
+      <c r="BO17" s="114"/>
+      <c r="BP17" s="114"/>
       <c r="BQ17" s="16"/>
       <c r="BR17" s="14"/>
       <c r="BS17" s="14"/>
@@ -4702,7 +4706,7 @@
       <c r="EV17" s="17"/>
     </row>
     <row r="18" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A18" s="107"/>
+      <c r="A18" s="123"/>
       <c r="B18" s="24"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -4765,11 +4769,11 @@
       <c r="BI18" s="14"/>
       <c r="BJ18" s="16"/>
       <c r="BK18" s="14"/>
-      <c r="BL18" s="125"/>
-      <c r="BM18" s="126"/>
-      <c r="BN18" s="125"/>
-      <c r="BO18" s="125"/>
-      <c r="BP18" s="125"/>
+      <c r="BL18" s="114"/>
+      <c r="BM18" s="115"/>
+      <c r="BN18" s="114"/>
+      <c r="BO18" s="114"/>
+      <c r="BP18" s="114"/>
       <c r="BQ18" s="16"/>
       <c r="BR18" s="14"/>
       <c r="BS18" s="14"/>
@@ -4858,7 +4862,7 @@
       <c r="EV18" s="17"/>
     </row>
     <row r="19" spans="1:152" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="107"/>
+      <c r="A19" s="123"/>
       <c r="B19" s="26"/>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
@@ -4921,11 +4925,11 @@
       <c r="BI19" s="20"/>
       <c r="BJ19" s="21"/>
       <c r="BK19" s="20"/>
-      <c r="BL19" s="127"/>
-      <c r="BM19" s="125"/>
-      <c r="BN19" s="127"/>
-      <c r="BO19" s="127"/>
-      <c r="BP19" s="127"/>
+      <c r="BL19" s="116"/>
+      <c r="BM19" s="114"/>
+      <c r="BN19" s="116"/>
+      <c r="BO19" s="116"/>
+      <c r="BP19" s="116"/>
       <c r="BQ19" s="21"/>
       <c r="BR19" s="20"/>
       <c r="BS19" s="20"/>
@@ -5014,7 +5018,7 @@
       <c r="EV19" s="99"/>
     </row>
     <row r="20" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="109" t="s">
+      <c r="A20" s="125" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="76"/>
@@ -5085,11 +5089,11 @@
       <c r="BI20" s="78"/>
       <c r="BJ20" s="77"/>
       <c r="BK20" s="78"/>
-      <c r="BL20" s="128"/>
-      <c r="BM20" s="128"/>
-      <c r="BN20" s="128"/>
-      <c r="BO20" s="129"/>
-      <c r="BP20" s="128"/>
+      <c r="BL20" s="117"/>
+      <c r="BM20" s="117"/>
+      <c r="BN20" s="117"/>
+      <c r="BO20" s="118"/>
+      <c r="BP20" s="117"/>
       <c r="BQ20" s="77"/>
       <c r="BR20" s="78"/>
       <c r="BS20" s="78"/>
@@ -5176,7 +5180,7 @@
       <c r="EV20" s="103"/>
     </row>
     <row r="21" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="107"/>
+      <c r="A21" s="123"/>
       <c r="B21" s="24"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -5243,11 +5247,11 @@
       <c r="BI21" s="14"/>
       <c r="BJ21" s="16"/>
       <c r="BK21" s="14"/>
-      <c r="BL21" s="125"/>
-      <c r="BM21" s="125"/>
-      <c r="BN21" s="125"/>
-      <c r="BO21" s="125"/>
-      <c r="BP21" s="125"/>
+      <c r="BL21" s="114"/>
+      <c r="BM21" s="114"/>
+      <c r="BN21" s="114"/>
+      <c r="BO21" s="114"/>
+      <c r="BP21" s="114"/>
       <c r="BQ21" s="16"/>
       <c r="BR21" s="14"/>
       <c r="BS21" s="14"/>
@@ -5334,7 +5338,7 @@
       <c r="EV21" s="17"/>
     </row>
     <row r="22" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="107"/>
+      <c r="A22" s="123"/>
       <c r="B22" s="24"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -5399,11 +5403,11 @@
       <c r="BI22" s="14"/>
       <c r="BJ22" s="16"/>
       <c r="BK22" s="14"/>
-      <c r="BL22" s="125"/>
-      <c r="BM22" s="125"/>
-      <c r="BN22" s="125"/>
-      <c r="BO22" s="125"/>
-      <c r="BP22" s="125"/>
+      <c r="BL22" s="114"/>
+      <c r="BM22" s="114"/>
+      <c r="BN22" s="114"/>
+      <c r="BO22" s="114"/>
+      <c r="BP22" s="114"/>
       <c r="BQ22" s="16"/>
       <c r="BR22" s="14"/>
       <c r="BS22" s="14"/>
@@ -5490,7 +5494,7 @@
       <c r="EV22" s="17"/>
     </row>
     <row r="23" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="107"/>
+      <c r="A23" s="123"/>
       <c r="B23" s="24"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
@@ -5537,7 +5541,9 @@
       <c r="AQ23" s="14"/>
       <c r="AR23" s="13"/>
       <c r="AS23" s="13"/>
-      <c r="AT23" s="13"/>
+      <c r="AT23" s="91" t="s">
+        <v>43</v>
+      </c>
       <c r="AU23" s="14"/>
       <c r="AV23" s="14"/>
       <c r="AW23" s="14"/>
@@ -5555,11 +5561,11 @@
       <c r="BI23" s="14"/>
       <c r="BJ23" s="13"/>
       <c r="BK23" s="14"/>
-      <c r="BL23" s="125"/>
-      <c r="BM23" s="125"/>
-      <c r="BN23" s="125"/>
-      <c r="BO23" s="125"/>
-      <c r="BP23" s="125"/>
+      <c r="BL23" s="114"/>
+      <c r="BM23" s="114"/>
+      <c r="BN23" s="114"/>
+      <c r="BO23" s="114"/>
+      <c r="BP23" s="114"/>
       <c r="BQ23" s="13"/>
       <c r="BR23" s="14"/>
       <c r="BS23" s="14"/>
@@ -5646,7 +5652,7 @@
       <c r="EV23" s="17"/>
     </row>
     <row r="24" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="108"/>
+      <c r="A24" s="124"/>
       <c r="B24" s="92"/>
       <c r="C24" s="93"/>
       <c r="D24" s="93"/>
@@ -5709,11 +5715,11 @@
       <c r="BI24" s="94"/>
       <c r="BJ24" s="93"/>
       <c r="BK24" s="94"/>
-      <c r="BL24" s="130"/>
-      <c r="BM24" s="130"/>
-      <c r="BN24" s="130"/>
-      <c r="BO24" s="130"/>
-      <c r="BP24" s="130"/>
+      <c r="BL24" s="119"/>
+      <c r="BM24" s="119"/>
+      <c r="BN24" s="119"/>
+      <c r="BO24" s="119"/>
+      <c r="BP24" s="119"/>
       <c r="BQ24" s="93"/>
       <c r="BR24" s="94"/>
       <c r="BS24" s="94"/>
@@ -5800,7 +5806,7 @@
       <c r="EV24" s="99"/>
     </row>
     <row r="25" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="109" t="s">
+      <c r="A25" s="125" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="76"/>
@@ -5865,11 +5871,11 @@
       <c r="BI25" s="78"/>
       <c r="BJ25" s="77"/>
       <c r="BK25" s="78"/>
-      <c r="BL25" s="128"/>
-      <c r="BM25" s="128"/>
-      <c r="BN25" s="128"/>
-      <c r="BO25" s="128"/>
-      <c r="BP25" s="128"/>
+      <c r="BL25" s="117"/>
+      <c r="BM25" s="117"/>
+      <c r="BN25" s="117"/>
+      <c r="BO25" s="117"/>
+      <c r="BP25" s="117"/>
       <c r="BQ25" s="77"/>
       <c r="BR25" s="78"/>
       <c r="BS25" s="78"/>
@@ -5956,7 +5962,7 @@
       <c r="EV25" s="103"/>
     </row>
     <row r="26" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="107"/>
+      <c r="A26" s="123"/>
       <c r="B26" s="24"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -6019,11 +6025,11 @@
       <c r="BI26" s="14"/>
       <c r="BJ26" s="16"/>
       <c r="BK26" s="14"/>
-      <c r="BL26" s="125"/>
-      <c r="BM26" s="125"/>
-      <c r="BN26" s="125"/>
-      <c r="BO26" s="125"/>
-      <c r="BP26" s="125"/>
+      <c r="BL26" s="114"/>
+      <c r="BM26" s="114"/>
+      <c r="BN26" s="114"/>
+      <c r="BO26" s="114"/>
+      <c r="BP26" s="114"/>
       <c r="BQ26" s="16"/>
       <c r="BR26" s="14"/>
       <c r="BS26" s="14"/>
@@ -6110,7 +6116,7 @@
       <c r="EV26" s="17"/>
     </row>
     <row r="27" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="107"/>
+      <c r="A27" s="123"/>
       <c r="B27" s="24"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
@@ -6173,11 +6179,11 @@
       <c r="BI27" s="14"/>
       <c r="BJ27" s="16"/>
       <c r="BK27" s="14"/>
-      <c r="BL27" s="125"/>
-      <c r="BM27" s="125"/>
-      <c r="BN27" s="125"/>
-      <c r="BO27" s="125"/>
-      <c r="BP27" s="125"/>
+      <c r="BL27" s="114"/>
+      <c r="BM27" s="114"/>
+      <c r="BN27" s="114"/>
+      <c r="BO27" s="114"/>
+      <c r="BP27" s="114"/>
       <c r="BQ27" s="16"/>
       <c r="BR27" s="14"/>
       <c r="BS27" s="14"/>
@@ -6264,7 +6270,7 @@
       <c r="EV27" s="17"/>
     </row>
     <row r="28" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="107"/>
+      <c r="A28" s="123"/>
       <c r="B28" s="24"/>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
@@ -6327,11 +6333,11 @@
       <c r="BI28" s="14"/>
       <c r="BJ28" s="16"/>
       <c r="BK28" s="14"/>
-      <c r="BL28" s="125"/>
-      <c r="BM28" s="125"/>
-      <c r="BN28" s="125"/>
-      <c r="BO28" s="125"/>
-      <c r="BP28" s="125"/>
+      <c r="BL28" s="114"/>
+      <c r="BM28" s="114"/>
+      <c r="BN28" s="114"/>
+      <c r="BO28" s="114"/>
+      <c r="BP28" s="114"/>
       <c r="BQ28" s="16"/>
       <c r="BR28" s="14"/>
       <c r="BS28" s="14"/>
@@ -6418,7 +6424,7 @@
       <c r="EV28" s="17"/>
     </row>
     <row r="29" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="107"/>
+      <c r="A29" s="123"/>
       <c r="B29" s="86"/>
       <c r="C29" s="72"/>
       <c r="D29" s="72"/>
@@ -6481,11 +6487,11 @@
       <c r="BI29" s="73"/>
       <c r="BJ29" s="72"/>
       <c r="BK29" s="73"/>
-      <c r="BL29" s="131"/>
-      <c r="BM29" s="131"/>
-      <c r="BN29" s="131"/>
-      <c r="BO29" s="131"/>
-      <c r="BP29" s="131"/>
+      <c r="BL29" s="120"/>
+      <c r="BM29" s="120"/>
+      <c r="BN29" s="120"/>
+      <c r="BO29" s="120"/>
+      <c r="BP29" s="120"/>
       <c r="BQ29" s="72"/>
       <c r="BR29" s="73"/>
       <c r="BS29" s="73"/>
@@ -6572,7 +6578,7 @@
       <c r="EV29" s="99"/>
     </row>
     <row r="30" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="106" t="s">
+      <c r="A30" s="122" t="s">
         <v>20</v>
       </c>
       <c r="B30" s="76"/>
@@ -6643,13 +6649,13 @@
       <c r="BI30" s="78"/>
       <c r="BJ30" s="77"/>
       <c r="BK30" s="78"/>
-      <c r="BL30" s="128"/>
-      <c r="BM30" s="132" t="s">
+      <c r="BL30" s="117"/>
+      <c r="BM30" s="121" t="s">
         <v>9</v>
       </c>
-      <c r="BN30" s="128"/>
-      <c r="BO30" s="128"/>
-      <c r="BP30" s="128"/>
+      <c r="BN30" s="117"/>
+      <c r="BO30" s="117"/>
+      <c r="BP30" s="117"/>
       <c r="BQ30" s="77"/>
       <c r="BR30" s="78"/>
       <c r="BS30" s="78"/>
@@ -6738,7 +6744,7 @@
       <c r="EV30" s="103"/>
     </row>
     <row r="31" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="107"/>
+      <c r="A31" s="123"/>
       <c r="B31" s="24"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
@@ -6803,11 +6809,11 @@
       <c r="BI31" s="14"/>
       <c r="BJ31" s="16"/>
       <c r="BK31" s="14"/>
-      <c r="BL31" s="125"/>
-      <c r="BM31" s="125"/>
-      <c r="BN31" s="125"/>
-      <c r="BO31" s="125"/>
-      <c r="BP31" s="125"/>
+      <c r="BL31" s="114"/>
+      <c r="BM31" s="114"/>
+      <c r="BN31" s="114"/>
+      <c r="BO31" s="114"/>
+      <c r="BP31" s="114"/>
       <c r="BQ31" s="16"/>
       <c r="BR31" s="14"/>
       <c r="BS31" s="14"/>
@@ -6896,7 +6902,7 @@
       <c r="EV31" s="17"/>
     </row>
     <row r="32" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="107"/>
+      <c r="A32" s="123"/>
       <c r="B32" s="24"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
@@ -6959,11 +6965,11 @@
       <c r="BI32" s="14"/>
       <c r="BJ32" s="16"/>
       <c r="BK32" s="14"/>
-      <c r="BL32" s="125"/>
-      <c r="BM32" s="125"/>
-      <c r="BN32" s="125"/>
-      <c r="BO32" s="125"/>
-      <c r="BP32" s="125"/>
+      <c r="BL32" s="114"/>
+      <c r="BM32" s="114"/>
+      <c r="BN32" s="114"/>
+      <c r="BO32" s="114"/>
+      <c r="BP32" s="114"/>
       <c r="BQ32" s="16"/>
       <c r="BR32" s="14"/>
       <c r="BS32" s="14"/>
@@ -7054,7 +7060,7 @@
       <c r="EV32" s="17"/>
     </row>
     <row r="33" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="107"/>
+      <c r="A33" s="123"/>
       <c r="B33" s="24"/>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
@@ -7117,11 +7123,11 @@
       <c r="BI33" s="14"/>
       <c r="BJ33" s="16"/>
       <c r="BK33" s="14"/>
-      <c r="BL33" s="125"/>
-      <c r="BM33" s="125"/>
-      <c r="BN33" s="125"/>
-      <c r="BO33" s="125"/>
-      <c r="BP33" s="125"/>
+      <c r="BL33" s="114"/>
+      <c r="BM33" s="114"/>
+      <c r="BN33" s="114"/>
+      <c r="BO33" s="114"/>
+      <c r="BP33" s="114"/>
       <c r="BQ33" s="16"/>
       <c r="BR33" s="14"/>
       <c r="BS33" s="14"/>
@@ -7210,7 +7216,7 @@
       <c r="EV33" s="17"/>
     </row>
     <row r="34" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="108"/>
+      <c r="A34" s="124"/>
       <c r="B34" s="86"/>
       <c r="C34" s="72"/>
       <c r="D34" s="72"/>
@@ -7273,11 +7279,11 @@
       <c r="BI34" s="73"/>
       <c r="BJ34" s="72"/>
       <c r="BK34" s="73"/>
-      <c r="BL34" s="131"/>
-      <c r="BM34" s="131"/>
-      <c r="BN34" s="131"/>
-      <c r="BO34" s="131"/>
-      <c r="BP34" s="131"/>
+      <c r="BL34" s="120"/>
+      <c r="BM34" s="120"/>
+      <c r="BN34" s="120"/>
+      <c r="BO34" s="120"/>
+      <c r="BP34" s="120"/>
       <c r="BQ34" s="72"/>
       <c r="BR34" s="73"/>
       <c r="BS34" s="73"/>
@@ -7366,7 +7372,7 @@
       <c r="EV34" s="99"/>
     </row>
     <row r="35" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="107" t="s">
+      <c r="A35" s="123" t="s">
         <v>23</v>
       </c>
       <c r="B35" s="76"/>
@@ -7433,11 +7439,11 @@
       <c r="BI35" s="78"/>
       <c r="BJ35" s="77"/>
       <c r="BK35" s="78"/>
-      <c r="BL35" s="128"/>
-      <c r="BM35" s="128"/>
-      <c r="BN35" s="128"/>
-      <c r="BO35" s="128"/>
-      <c r="BP35" s="128"/>
+      <c r="BL35" s="117"/>
+      <c r="BM35" s="117"/>
+      <c r="BN35" s="117"/>
+      <c r="BO35" s="117"/>
+      <c r="BP35" s="117"/>
       <c r="BQ35" s="77"/>
       <c r="BR35" s="78"/>
       <c r="BS35" s="78"/>
@@ -7524,7 +7530,7 @@
       <c r="EV35" s="103"/>
     </row>
     <row r="36" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="107"/>
+      <c r="A36" s="123"/>
       <c r="B36" s="24"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16"/>
@@ -7589,11 +7595,11 @@
       <c r="BI36" s="14"/>
       <c r="BJ36" s="16"/>
       <c r="BK36" s="14"/>
-      <c r="BL36" s="125"/>
-      <c r="BM36" s="125"/>
-      <c r="BN36" s="125"/>
-      <c r="BO36" s="125"/>
-      <c r="BP36" s="125"/>
+      <c r="BL36" s="114"/>
+      <c r="BM36" s="114"/>
+      <c r="BN36" s="114"/>
+      <c r="BO36" s="114"/>
+      <c r="BP36" s="114"/>
       <c r="BQ36" s="16"/>
       <c r="BR36" s="14"/>
       <c r="BS36" s="14"/>
@@ -7680,7 +7686,7 @@
       <c r="EV36" s="17"/>
     </row>
     <row r="37" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="107"/>
+      <c r="A37" s="123"/>
       <c r="B37" s="24"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
@@ -7743,11 +7749,11 @@
       <c r="BI37" s="14"/>
       <c r="BJ37" s="16"/>
       <c r="BK37" s="14"/>
-      <c r="BL37" s="125"/>
-      <c r="BM37" s="125"/>
-      <c r="BN37" s="125"/>
-      <c r="BO37" s="125"/>
-      <c r="BP37" s="125"/>
+      <c r="BL37" s="114"/>
+      <c r="BM37" s="114"/>
+      <c r="BN37" s="114"/>
+      <c r="BO37" s="114"/>
+      <c r="BP37" s="114"/>
       <c r="BQ37" s="16"/>
       <c r="BR37" s="14"/>
       <c r="BS37" s="14"/>
@@ -7834,7 +7840,7 @@
       <c r="EV37" s="17"/>
     </row>
     <row r="38" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="107"/>
+      <c r="A38" s="123"/>
       <c r="B38" s="24"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
@@ -7897,11 +7903,11 @@
       <c r="BI38" s="14"/>
       <c r="BJ38" s="16"/>
       <c r="BK38" s="14"/>
-      <c r="BL38" s="125"/>
-      <c r="BM38" s="125"/>
-      <c r="BN38" s="125"/>
-      <c r="BO38" s="125"/>
-      <c r="BP38" s="125"/>
+      <c r="BL38" s="114"/>
+      <c r="BM38" s="114"/>
+      <c r="BN38" s="114"/>
+      <c r="BO38" s="114"/>
+      <c r="BP38" s="114"/>
       <c r="BQ38" s="16"/>
       <c r="BR38" s="14"/>
       <c r="BS38" s="14"/>
@@ -7988,7 +7994,7 @@
       <c r="EV38" s="17"/>
     </row>
     <row r="39" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="107"/>
+      <c r="A39" s="123"/>
       <c r="B39" s="86"/>
       <c r="C39" s="72"/>
       <c r="D39" s="72"/>
@@ -8051,11 +8057,11 @@
       <c r="BI39" s="73"/>
       <c r="BJ39" s="72"/>
       <c r="BK39" s="73"/>
-      <c r="BL39" s="131"/>
-      <c r="BM39" s="131"/>
-      <c r="BN39" s="131"/>
-      <c r="BO39" s="131"/>
-      <c r="BP39" s="131"/>
+      <c r="BL39" s="120"/>
+      <c r="BM39" s="120"/>
+      <c r="BN39" s="120"/>
+      <c r="BO39" s="120"/>
+      <c r="BP39" s="120"/>
       <c r="BQ39" s="72"/>
       <c r="BR39" s="73"/>
       <c r="BS39" s="73"/>
@@ -8142,7 +8148,7 @@
       <c r="EV39" s="99"/>
     </row>
     <row r="40" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="106" t="s">
+      <c r="A40" s="122" t="s">
         <v>22</v>
       </c>
       <c r="B40" s="76"/>
@@ -8211,11 +8217,11 @@
       <c r="BI40" s="78"/>
       <c r="BJ40" s="77"/>
       <c r="BK40" s="78"/>
-      <c r="BL40" s="128"/>
-      <c r="BM40" s="132"/>
-      <c r="BN40" s="128"/>
-      <c r="BO40" s="128"/>
-      <c r="BP40" s="128"/>
+      <c r="BL40" s="117"/>
+      <c r="BM40" s="121"/>
+      <c r="BN40" s="117"/>
+      <c r="BO40" s="117"/>
+      <c r="BP40" s="117"/>
       <c r="BQ40" s="77"/>
       <c r="BR40" s="78"/>
       <c r="BS40" s="78"/>
@@ -8304,7 +8310,7 @@
       <c r="EV40" s="103"/>
     </row>
     <row r="41" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="107"/>
+      <c r="A41" s="123"/>
       <c r="B41" s="24"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
@@ -8367,11 +8373,11 @@
       <c r="BI41" s="14"/>
       <c r="BJ41" s="16"/>
       <c r="BK41" s="14"/>
-      <c r="BL41" s="125"/>
-      <c r="BM41" s="125"/>
-      <c r="BN41" s="125"/>
-      <c r="BO41" s="125"/>
-      <c r="BP41" s="125"/>
+      <c r="BL41" s="114"/>
+      <c r="BM41" s="114"/>
+      <c r="BN41" s="114"/>
+      <c r="BO41" s="114"/>
+      <c r="BP41" s="114"/>
       <c r="BQ41" s="16"/>
       <c r="BR41" s="14"/>
       <c r="BS41" s="14"/>
@@ -8460,7 +8466,7 @@
       <c r="EV41" s="17"/>
     </row>
     <row r="42" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="107"/>
+      <c r="A42" s="123"/>
       <c r="B42" s="24"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
@@ -8523,11 +8529,11 @@
       <c r="BI42" s="14"/>
       <c r="BJ42" s="16"/>
       <c r="BK42" s="14"/>
-      <c r="BL42" s="125"/>
-      <c r="BM42" s="125"/>
-      <c r="BN42" s="125"/>
-      <c r="BO42" s="125"/>
-      <c r="BP42" s="125"/>
+      <c r="BL42" s="114"/>
+      <c r="BM42" s="114"/>
+      <c r="BN42" s="114"/>
+      <c r="BO42" s="114"/>
+      <c r="BP42" s="114"/>
       <c r="BQ42" s="16"/>
       <c r="BR42" s="14"/>
       <c r="BS42" s="14"/>
@@ -8618,7 +8624,7 @@
       <c r="EV42" s="17"/>
     </row>
     <row r="43" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="107"/>
+      <c r="A43" s="123"/>
       <c r="B43" s="24"/>
       <c r="C43" s="16"/>
       <c r="D43" s="16"/>
@@ -8681,11 +8687,11 @@
       <c r="BI43" s="14"/>
       <c r="BJ43" s="16"/>
       <c r="BK43" s="14"/>
-      <c r="BL43" s="125"/>
-      <c r="BM43" s="125"/>
-      <c r="BN43" s="125"/>
-      <c r="BO43" s="125"/>
-      <c r="BP43" s="125"/>
+      <c r="BL43" s="114"/>
+      <c r="BM43" s="114"/>
+      <c r="BN43" s="114"/>
+      <c r="BO43" s="114"/>
+      <c r="BP43" s="114"/>
       <c r="BQ43" s="16"/>
       <c r="BR43" s="14"/>
       <c r="BS43" s="14"/>
@@ -8774,7 +8780,7 @@
       <c r="EV43" s="17"/>
     </row>
     <row r="44" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="108"/>
+      <c r="A44" s="124"/>
       <c r="B44" s="86"/>
       <c r="C44" s="72"/>
       <c r="D44" s="72"/>
@@ -8837,11 +8843,11 @@
       <c r="BI44" s="73"/>
       <c r="BJ44" s="72"/>
       <c r="BK44" s="73"/>
-      <c r="BL44" s="131"/>
-      <c r="BM44" s="131"/>
-      <c r="BN44" s="131"/>
-      <c r="BO44" s="131"/>
-      <c r="BP44" s="131"/>
+      <c r="BL44" s="120"/>
+      <c r="BM44" s="120"/>
+      <c r="BN44" s="120"/>
+      <c r="BO44" s="120"/>
+      <c r="BP44" s="120"/>
       <c r="BQ44" s="72"/>
       <c r="BR44" s="73"/>
       <c r="BS44" s="73"/>
@@ -8930,7 +8936,7 @@
       <c r="EV44" s="99"/>
     </row>
     <row r="45" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="107" t="s">
+      <c r="A45" s="123" t="s">
         <v>24</v>
       </c>
       <c r="B45" s="76"/>
@@ -8999,11 +9005,11 @@
       <c r="BI45" s="78"/>
       <c r="BJ45" s="77"/>
       <c r="BK45" s="78"/>
-      <c r="BL45" s="128"/>
-      <c r="BM45" s="128"/>
-      <c r="BN45" s="128"/>
-      <c r="BO45" s="128"/>
-      <c r="BP45" s="128"/>
+      <c r="BL45" s="117"/>
+      <c r="BM45" s="117"/>
+      <c r="BN45" s="117"/>
+      <c r="BO45" s="117"/>
+      <c r="BP45" s="117"/>
       <c r="BQ45" s="77"/>
       <c r="BR45" s="78"/>
       <c r="BS45" s="78"/>
@@ -9092,7 +9098,7 @@
       <c r="EV45" s="103"/>
     </row>
     <row r="46" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="107"/>
+      <c r="A46" s="123"/>
       <c r="B46" s="24"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
@@ -9155,11 +9161,11 @@
       <c r="BI46" s="14"/>
       <c r="BJ46" s="16"/>
       <c r="BK46" s="14"/>
-      <c r="BL46" s="125"/>
-      <c r="BM46" s="125"/>
-      <c r="BN46" s="125"/>
-      <c r="BO46" s="125"/>
-      <c r="BP46" s="125"/>
+      <c r="BL46" s="114"/>
+      <c r="BM46" s="114"/>
+      <c r="BN46" s="114"/>
+      <c r="BO46" s="114"/>
+      <c r="BP46" s="114"/>
       <c r="BQ46" s="16"/>
       <c r="BR46" s="14"/>
       <c r="BS46" s="14"/>
@@ -9248,7 +9254,7 @@
       <c r="EV46" s="17"/>
     </row>
     <row r="47" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="107"/>
+      <c r="A47" s="123"/>
       <c r="B47" s="24"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
@@ -9311,11 +9317,11 @@
       <c r="BI47" s="14"/>
       <c r="BJ47" s="16"/>
       <c r="BK47" s="14"/>
-      <c r="BL47" s="125"/>
-      <c r="BM47" s="125"/>
-      <c r="BN47" s="125"/>
-      <c r="BO47" s="125"/>
-      <c r="BP47" s="125"/>
+      <c r="BL47" s="114"/>
+      <c r="BM47" s="114"/>
+      <c r="BN47" s="114"/>
+      <c r="BO47" s="114"/>
+      <c r="BP47" s="114"/>
       <c r="BQ47" s="16"/>
       <c r="BR47" s="14"/>
       <c r="BS47" s="14"/>
@@ -9406,7 +9412,7 @@
       <c r="EV47" s="17"/>
     </row>
     <row r="48" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="107"/>
+      <c r="A48" s="123"/>
       <c r="B48" s="24"/>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
@@ -9469,11 +9475,11 @@
       <c r="BI48" s="14"/>
       <c r="BJ48" s="16"/>
       <c r="BK48" s="14"/>
-      <c r="BL48" s="125"/>
-      <c r="BM48" s="125"/>
-      <c r="BN48" s="125"/>
-      <c r="BO48" s="125"/>
-      <c r="BP48" s="125"/>
+      <c r="BL48" s="114"/>
+      <c r="BM48" s="114"/>
+      <c r="BN48" s="114"/>
+      <c r="BO48" s="114"/>
+      <c r="BP48" s="114"/>
       <c r="BQ48" s="16"/>
       <c r="BR48" s="14"/>
       <c r="BS48" s="14"/>
@@ -9562,7 +9568,7 @@
       <c r="EV48" s="17"/>
     </row>
     <row r="49" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="108"/>
+      <c r="A49" s="124"/>
       <c r="B49" s="86"/>
       <c r="C49" s="72"/>
       <c r="D49" s="72"/>
@@ -9625,11 +9631,11 @@
       <c r="BI49" s="73"/>
       <c r="BJ49" s="72"/>
       <c r="BK49" s="73"/>
-      <c r="BL49" s="131"/>
-      <c r="BM49" s="131"/>
-      <c r="BN49" s="131"/>
-      <c r="BO49" s="131"/>
-      <c r="BP49" s="131"/>
+      <c r="BL49" s="120"/>
+      <c r="BM49" s="120"/>
+      <c r="BN49" s="120"/>
+      <c r="BO49" s="120"/>
+      <c r="BP49" s="120"/>
       <c r="BQ49" s="72"/>
       <c r="BR49" s="73"/>
       <c r="BS49" s="73"/>

</xml_diff>

<commit_message>
[Pipette] Transformer 부품 입고 update
</commit_message>
<xml_diff>
--- a/0_DOC/Femto Project schedule V1.0.xlsx
+++ b/0_DOC/Femto Project schedule V1.0.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
   <si>
     <t>◇PCB설계</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -192,6 +192,22 @@
   </si>
   <si>
     <t>◇PCB 입고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>◇1,2차 부품 입고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>▶업체 방문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LF 불량보드 입수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LF 운용 설명 및 시연</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1021,16 +1037,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>57</xdr:col>
-      <xdr:colOff>148258</xdr:colOff>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>186358</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>107311</xdr:rowOff>
+      <xdr:rowOff>97786</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>60</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:col>69</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>107311</xdr:rowOff>
+      <xdr:rowOff>97786</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1039,8 +1055,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12539041" y="3503181"/>
-          <a:ext cx="448090" cy="0"/>
+          <a:off x="13816633" y="3650611"/>
+          <a:ext cx="823292" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1078,8 +1094,8 @@
       <xdr:rowOff>94059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>45</xdr:col>
-      <xdr:colOff>165652</xdr:colOff>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>94059</xdr:rowOff>
     </xdr:to>
@@ -1090,8 +1106,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9237594" y="3332559"/>
-          <a:ext cx="933449" cy="0"/>
+          <a:off x="9057033" y="3818334"/>
+          <a:ext cx="2315817" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2466,8 +2482,8 @@
   <dimension ref="A1:EV66"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BB27" sqref="BB27"/>
+      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BV27" sqref="BV27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3188,7 +3204,9 @@
       <c r="BD8" s="38"/>
       <c r="BE8" s="38"/>
       <c r="BF8" s="50"/>
-      <c r="BG8" s="35"/>
+      <c r="BG8" s="42" t="s">
+        <v>45</v>
+      </c>
       <c r="BH8" s="63"/>
       <c r="BI8" s="38"/>
       <c r="BJ8" s="35"/>
@@ -3347,7 +3365,9 @@
       <c r="BE9" s="31"/>
       <c r="BF9" s="28"/>
       <c r="BG9" s="30"/>
-      <c r="BH9" s="32"/>
+      <c r="BH9" s="32" t="s">
+        <v>46</v>
+      </c>
       <c r="BI9" s="31"/>
       <c r="BJ9" s="30"/>
       <c r="BK9" s="31"/>
@@ -3505,7 +3525,9 @@
       <c r="BE10" s="31"/>
       <c r="BF10" s="28"/>
       <c r="BG10" s="30"/>
-      <c r="BH10" s="32"/>
+      <c r="BH10" s="32" t="s">
+        <v>47</v>
+      </c>
       <c r="BI10" s="31"/>
       <c r="BJ10" s="30"/>
       <c r="BK10" s="31"/>
@@ -5071,22 +5093,22 @@
       <c r="AU20" s="78"/>
       <c r="AV20" s="78"/>
       <c r="AW20" s="78"/>
-      <c r="AX20" s="40" t="s">
-        <v>18</v>
-      </c>
+      <c r="AX20" s="78"/>
       <c r="AY20" s="77"/>
       <c r="AZ20" s="77"/>
       <c r="BA20" s="87"/>
       <c r="BB20" s="77"/>
-      <c r="BC20" s="77"/>
-      <c r="BD20" s="89" t="s">
-        <v>19</v>
-      </c>
-      <c r="BE20" s="89"/>
+      <c r="BC20" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="BD20" s="78"/>
+      <c r="BE20" s="78"/>
       <c r="BF20" s="77"/>
       <c r="BG20" s="77"/>
       <c r="BH20" s="90"/>
-      <c r="BI20" s="78"/>
+      <c r="BI20" s="89" t="s">
+        <v>19</v>
+      </c>
       <c r="BJ20" s="77"/>
       <c r="BK20" s="78"/>
       <c r="BL20" s="117"/>
@@ -5232,16 +5254,16 @@
       <c r="AV21" s="14"/>
       <c r="AW21" s="14"/>
       <c r="AX21" s="14"/>
-      <c r="AY21" s="23" t="s">
-        <v>2</v>
-      </c>
+      <c r="AY21" s="23"/>
       <c r="AZ21" s="16"/>
       <c r="BA21" s="16"/>
       <c r="BB21" s="16"/>
       <c r="BC21" s="16"/>
       <c r="BD21" s="14"/>
       <c r="BE21" s="14"/>
-      <c r="BF21" s="16"/>
+      <c r="BF21" s="23" t="s">
+        <v>2</v>
+      </c>
       <c r="BG21" s="16"/>
       <c r="BH21" s="25"/>
       <c r="BI21" s="14"/>
@@ -5393,7 +5415,9 @@
       <c r="AY22" s="16"/>
       <c r="AZ22" s="16"/>
       <c r="BA22" s="16"/>
-      <c r="BB22" s="16"/>
+      <c r="BB22" s="91" t="s">
+        <v>44</v>
+      </c>
       <c r="BC22" s="16"/>
       <c r="BD22" s="14"/>
       <c r="BE22" s="14"/>

</xml_diff>

<commit_message>
[Pipett] 하네스 BOM 및 Datasheet update
</commit_message>
<xml_diff>
--- a/0_DOC/Femto Project schedule V1.0.xlsx
+++ b/0_DOC/Femto Project schedule V1.0.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="1"/>
@@ -12,14 +12,69 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'20180207'!$A$1:$EH$49</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'20180328'!$A$1:$EH$49</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'20180328'!$A$1:$FZ$49</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>만든 이</author>
+  </authors>
+  <commentList>
+    <comment ref="EM7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>석가탄신일</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FB7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>현충일</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FI7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>지방선거</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="68">
   <si>
     <t>◇PCB설계</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -253,10 +308,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>◇회로Tuning&amp;debugging</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>◇일부 부품발주(12일)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -288,12 +339,20 @@
     <t>◇PCB제작(3ea)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>◇PCB제작(10ea)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>◇회로Tuning&amp;debugging</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,6 +432,14 @@
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="6">
@@ -910,7 +977,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1088,6 +1155,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -2669,8 +2760,8 @@
       <xdr:rowOff>94059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>100</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:col>122</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>94059</xdr:rowOff>
     </xdr:to>
@@ -2681,8 +2772,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1028700" y="6904434"/>
-          <a:ext cx="8153400" cy="0"/>
+          <a:off x="1028700" y="6218634"/>
+          <a:ext cx="12592050" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3148,7 +3239,7 @@
         </a:prstGeom>
         <a:ln w="28575">
           <a:solidFill>
-            <a:srgbClr val="0070C0"/>
+            <a:sysClr val="windowText" lastClr="000000"/>
           </a:solidFill>
           <a:prstDash val="sysDash"/>
           <a:tailEnd type="triangle"/>
@@ -3199,7 +3290,7 @@
         </a:prstGeom>
         <a:ln w="28575">
           <a:solidFill>
-            <a:srgbClr val="0070C0"/>
+            <a:sysClr val="windowText" lastClr="000000"/>
           </a:solidFill>
           <a:prstDash val="sysDash"/>
           <a:tailEnd type="triangle"/>
@@ -3377,159 +3468,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>161</xdr:col>
-      <xdr:colOff>75787</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>94888</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>168</xdr:col>
-      <xdr:colOff>22363</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>94888</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="59" name="직선 화살표 연결선 58"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="21307012" y="6905263"/>
-          <a:ext cx="1346751" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:srgbClr val="0070C0"/>
-          </a:solidFill>
-          <a:prstDash val="sysDash"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>162</xdr:col>
-      <xdr:colOff>28162</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>75838</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>168</xdr:col>
-      <xdr:colOff>174763</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>75838</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="60" name="직선 화살표 연결선 59"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="21459412" y="7057663"/>
-          <a:ext cx="1346751" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:srgbClr val="0070C0"/>
-          </a:solidFill>
-          <a:prstDash val="sysDash"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>162</xdr:col>
-      <xdr:colOff>180562</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>56788</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>169</xdr:col>
-      <xdr:colOff>127138</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>56788</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="61" name="직선 화살표 연결선 60"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="21611812" y="7210063"/>
-          <a:ext cx="1346751" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:srgbClr val="0070C0"/>
-          </a:solidFill>
-          <a:prstDash val="sysDash"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>105</xdr:col>
       <xdr:colOff>115544</xdr:colOff>
       <xdr:row>32</xdr:row>
@@ -3549,57 +3487,6 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10145369" y="5704285"/>
-          <a:ext cx="856006" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:srgbClr val="0070C0"/>
-          </a:solidFill>
-          <a:prstDash val="sysDash"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>110</xdr:col>
-      <xdr:colOff>106019</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>94060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>114</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>94060</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="68" name="직선 화살표 연결선 67"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11135969" y="7418785"/>
           <a:ext cx="856006" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -3684,24 +3571,24 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>106</xdr:col>
-      <xdr:colOff>20294</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>94060</xdr:rowOff>
+      <xdr:colOff>10769</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>103585</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>112</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>94060</xdr:rowOff>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>103585</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="72" name="직선 화살표 연결선 71"/>
+        <xdr:cNvPr id="74" name="직선 화살표 연결선 73"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10250144" y="7247335"/>
+          <a:off x="10240619" y="5542360"/>
           <a:ext cx="1360831" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -3734,26 +3621,179 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>106</xdr:col>
-      <xdr:colOff>10769</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:col>96</xdr:col>
+      <xdr:colOff>106019</xdr:colOff>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>103585</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>112</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:col>100</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>103585</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="74" name="직선 화살표 연결선 73"/>
+        <xdr:cNvPr id="31" name="직선 화살표 연결선 30"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10240619" y="5542360"/>
+          <a:off x="8335619" y="3313510"/>
+          <a:ext cx="856006" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>132</xdr:col>
+      <xdr:colOff>125069</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>84535</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>136</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>84535</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="직선 화살표 연결선 33"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15555569" y="6723460"/>
+          <a:ext cx="856006" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>133</xdr:col>
+      <xdr:colOff>20294</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>94060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>139</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>94060</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="직선 화살표 연결선 35"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15650819" y="6561535"/>
           <a:ext cx="1360831" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>117</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>99858</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>132</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>99858</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="직선 화살표 연결선 36"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12601575" y="5195733"/>
+          <a:ext cx="2971800" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3829,7 +3869,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3864,7 +3904,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -11380,47 +11420,47 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EV66"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:FZ66"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DK41" sqref="DK41"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="BJ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DK28" sqref="DK28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="60" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="2" max="60" width="2.625" style="2" hidden="1" customWidth="1"/>
     <col min="61" max="16384" width="2.625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:152" s="4" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:182" s="4" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:152" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:182" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:152" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:182" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:152" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:182" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="104" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:152" s="4" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:182" s="4" customFormat="1" ht="14.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="103" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:152" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:182" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="129">
         <v>1</v>
@@ -11583,8 +11623,40 @@
       <c r="ET6" s="126"/>
       <c r="EU6" s="126"/>
       <c r="EV6" s="127"/>
+      <c r="EW6" s="130">
+        <v>6</v>
+      </c>
+      <c r="EX6" s="131"/>
+      <c r="EY6" s="131"/>
+      <c r="EZ6" s="131"/>
+      <c r="FA6" s="131"/>
+      <c r="FB6" s="131"/>
+      <c r="FC6" s="131"/>
+      <c r="FD6" s="131"/>
+      <c r="FE6" s="131"/>
+      <c r="FF6" s="131"/>
+      <c r="FG6" s="131"/>
+      <c r="FH6" s="131"/>
+      <c r="FI6" s="131"/>
+      <c r="FJ6" s="131"/>
+      <c r="FK6" s="131"/>
+      <c r="FL6" s="131"/>
+      <c r="FM6" s="131"/>
+      <c r="FN6" s="131"/>
+      <c r="FO6" s="131"/>
+      <c r="FP6" s="131"/>
+      <c r="FQ6" s="131"/>
+      <c r="FR6" s="131"/>
+      <c r="FS6" s="131"/>
+      <c r="FT6" s="131"/>
+      <c r="FU6" s="131"/>
+      <c r="FV6" s="131"/>
+      <c r="FW6" s="131"/>
+      <c r="FX6" s="131"/>
+      <c r="FY6" s="131"/>
+      <c r="FZ6" s="132"/>
     </row>
-    <row r="7" spans="1:152" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:182" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="11">
         <v>1</v>
@@ -12039,8 +12111,98 @@
       <c r="EV7" s="9">
         <v>31</v>
       </c>
+      <c r="EW7" s="137">
+        <v>1</v>
+      </c>
+      <c r="EX7" s="1">
+        <v>2</v>
+      </c>
+      <c r="EY7" s="1">
+        <v>3</v>
+      </c>
+      <c r="EZ7" s="6">
+        <v>4</v>
+      </c>
+      <c r="FA7" s="6">
+        <v>5</v>
+      </c>
+      <c r="FB7" s="1">
+        <v>6</v>
+      </c>
+      <c r="FC7" s="6">
+        <v>7</v>
+      </c>
+      <c r="FD7" s="6">
+        <v>8</v>
+      </c>
+      <c r="FE7" s="1">
+        <v>9</v>
+      </c>
+      <c r="FF7" s="1">
+        <v>10</v>
+      </c>
+      <c r="FG7" s="6">
+        <v>11</v>
+      </c>
+      <c r="FH7" s="6">
+        <v>12</v>
+      </c>
+      <c r="FI7" s="1">
+        <v>13</v>
+      </c>
+      <c r="FJ7" s="6">
+        <v>14</v>
+      </c>
+      <c r="FK7" s="6">
+        <v>15</v>
+      </c>
+      <c r="FL7" s="1">
+        <v>16</v>
+      </c>
+      <c r="FM7" s="1">
+        <v>17</v>
+      </c>
+      <c r="FN7" s="6">
+        <v>18</v>
+      </c>
+      <c r="FO7" s="6">
+        <v>19</v>
+      </c>
+      <c r="FP7" s="6">
+        <v>20</v>
+      </c>
+      <c r="FQ7" s="6">
+        <v>21</v>
+      </c>
+      <c r="FR7" s="6">
+        <v>22</v>
+      </c>
+      <c r="FS7" s="1">
+        <v>23</v>
+      </c>
+      <c r="FT7" s="1">
+        <v>24</v>
+      </c>
+      <c r="FU7" s="6">
+        <v>25</v>
+      </c>
+      <c r="FV7" s="6">
+        <v>26</v>
+      </c>
+      <c r="FW7" s="6">
+        <v>27</v>
+      </c>
+      <c r="FX7" s="6">
+        <v>28</v>
+      </c>
+      <c r="FY7" s="6">
+        <v>29</v>
+      </c>
+      <c r="FZ7" s="144">
+        <v>30</v>
+      </c>
     </row>
-    <row r="8" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:182" x14ac:dyDescent="0.25">
       <c r="A8" s="123" t="s">
         <v>8</v>
       </c>
@@ -12207,8 +12369,38 @@
       <c r="ET8" s="49"/>
       <c r="EU8" s="49"/>
       <c r="EV8" s="99"/>
+      <c r="EW8" s="35"/>
+      <c r="EX8" s="38"/>
+      <c r="EY8" s="38"/>
+      <c r="EZ8" s="49"/>
+      <c r="FA8" s="35"/>
+      <c r="FB8" s="38"/>
+      <c r="FC8" s="35"/>
+      <c r="FD8" s="35"/>
+      <c r="FE8" s="38"/>
+      <c r="FF8" s="38"/>
+      <c r="FG8" s="49"/>
+      <c r="FH8" s="35"/>
+      <c r="FI8" s="38"/>
+      <c r="FJ8" s="35"/>
+      <c r="FK8" s="35"/>
+      <c r="FL8" s="38"/>
+      <c r="FM8" s="38"/>
+      <c r="FN8" s="49"/>
+      <c r="FO8" s="35"/>
+      <c r="FP8" s="36"/>
+      <c r="FQ8" s="35"/>
+      <c r="FR8" s="35"/>
+      <c r="FS8" s="38"/>
+      <c r="FT8" s="38"/>
+      <c r="FU8" s="49"/>
+      <c r="FV8" s="35"/>
+      <c r="FW8" s="36"/>
+      <c r="FX8" s="35"/>
+      <c r="FY8" s="35"/>
+      <c r="FZ8" s="145"/>
     </row>
-    <row r="9" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:182" x14ac:dyDescent="0.25">
       <c r="A9" s="123"/>
       <c r="B9" s="29"/>
       <c r="C9" s="30"/>
@@ -12369,8 +12561,38 @@
       <c r="ET9" s="28"/>
       <c r="EU9" s="28"/>
       <c r="EV9" s="33"/>
+      <c r="EW9" s="63"/>
+      <c r="EX9" s="31"/>
+      <c r="EY9" s="31"/>
+      <c r="EZ9" s="30"/>
+      <c r="FA9" s="30"/>
+      <c r="FB9" s="31"/>
+      <c r="FC9" s="30"/>
+      <c r="FD9" s="30"/>
+      <c r="FE9" s="31"/>
+      <c r="FF9" s="31"/>
+      <c r="FG9" s="30"/>
+      <c r="FH9" s="30"/>
+      <c r="FI9" s="31"/>
+      <c r="FJ9" s="30"/>
+      <c r="FK9" s="30"/>
+      <c r="FL9" s="31"/>
+      <c r="FM9" s="31"/>
+      <c r="FN9" s="30"/>
+      <c r="FO9" s="30"/>
+      <c r="FP9" s="30"/>
+      <c r="FQ9" s="30"/>
+      <c r="FR9" s="30"/>
+      <c r="FS9" s="31"/>
+      <c r="FT9" s="31"/>
+      <c r="FU9" s="30"/>
+      <c r="FV9" s="30"/>
+      <c r="FW9" s="30"/>
+      <c r="FX9" s="30"/>
+      <c r="FY9" s="30"/>
+      <c r="FZ9" s="146"/>
     </row>
-    <row r="10" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:182" x14ac:dyDescent="0.25">
       <c r="A10" s="123"/>
       <c r="B10" s="29"/>
       <c r="C10" s="30"/>
@@ -12531,8 +12753,38 @@
       <c r="ET10" s="28"/>
       <c r="EU10" s="28"/>
       <c r="EV10" s="33"/>
+      <c r="EW10" s="63"/>
+      <c r="EX10" s="31"/>
+      <c r="EY10" s="31"/>
+      <c r="EZ10" s="30"/>
+      <c r="FA10" s="30"/>
+      <c r="FB10" s="31"/>
+      <c r="FC10" s="30"/>
+      <c r="FD10" s="30"/>
+      <c r="FE10" s="31"/>
+      <c r="FF10" s="31"/>
+      <c r="FG10" s="30"/>
+      <c r="FH10" s="30"/>
+      <c r="FI10" s="31"/>
+      <c r="FJ10" s="30"/>
+      <c r="FK10" s="30"/>
+      <c r="FL10" s="31"/>
+      <c r="FM10" s="31"/>
+      <c r="FN10" s="30"/>
+      <c r="FO10" s="30"/>
+      <c r="FP10" s="30"/>
+      <c r="FQ10" s="30"/>
+      <c r="FR10" s="30"/>
+      <c r="FS10" s="31"/>
+      <c r="FT10" s="31"/>
+      <c r="FU10" s="30"/>
+      <c r="FV10" s="30"/>
+      <c r="FW10" s="30"/>
+      <c r="FX10" s="30"/>
+      <c r="FY10" s="30"/>
+      <c r="FZ10" s="146"/>
     </row>
-    <row r="11" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:182" x14ac:dyDescent="0.25">
       <c r="A11" s="123"/>
       <c r="B11" s="29"/>
       <c r="C11" s="30"/>
@@ -12689,8 +12941,38 @@
       <c r="ET11" s="28"/>
       <c r="EU11" s="28"/>
       <c r="EV11" s="33"/>
+      <c r="EW11" s="63"/>
+      <c r="EX11" s="31"/>
+      <c r="EY11" s="31"/>
+      <c r="EZ11" s="30"/>
+      <c r="FA11" s="30"/>
+      <c r="FB11" s="31"/>
+      <c r="FC11" s="30"/>
+      <c r="FD11" s="30"/>
+      <c r="FE11" s="31"/>
+      <c r="FF11" s="31"/>
+      <c r="FG11" s="30"/>
+      <c r="FH11" s="30"/>
+      <c r="FI11" s="31"/>
+      <c r="FJ11" s="30"/>
+      <c r="FK11" s="30"/>
+      <c r="FL11" s="31"/>
+      <c r="FM11" s="31"/>
+      <c r="FN11" s="30"/>
+      <c r="FO11" s="30"/>
+      <c r="FP11" s="30"/>
+      <c r="FQ11" s="30"/>
+      <c r="FR11" s="30"/>
+      <c r="FS11" s="31"/>
+      <c r="FT11" s="31"/>
+      <c r="FU11" s="30"/>
+      <c r="FV11" s="30"/>
+      <c r="FW11" s="30"/>
+      <c r="FX11" s="30"/>
+      <c r="FY11" s="30"/>
+      <c r="FZ11" s="146"/>
     </row>
-    <row r="12" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:182" x14ac:dyDescent="0.25">
       <c r="A12" s="123"/>
       <c r="B12" s="29"/>
       <c r="C12" s="30"/>
@@ -12847,8 +13129,38 @@
       <c r="ET12" s="28"/>
       <c r="EU12" s="28"/>
       <c r="EV12" s="33"/>
+      <c r="EW12" s="63"/>
+      <c r="EX12" s="31"/>
+      <c r="EY12" s="31"/>
+      <c r="EZ12" s="30"/>
+      <c r="FA12" s="30"/>
+      <c r="FB12" s="31"/>
+      <c r="FC12" s="30"/>
+      <c r="FD12" s="30"/>
+      <c r="FE12" s="31"/>
+      <c r="FF12" s="31"/>
+      <c r="FG12" s="30"/>
+      <c r="FH12" s="30"/>
+      <c r="FI12" s="31"/>
+      <c r="FJ12" s="30"/>
+      <c r="FK12" s="30"/>
+      <c r="FL12" s="31"/>
+      <c r="FM12" s="31"/>
+      <c r="FN12" s="30"/>
+      <c r="FO12" s="30"/>
+      <c r="FP12" s="30"/>
+      <c r="FQ12" s="30"/>
+      <c r="FR12" s="30"/>
+      <c r="FS12" s="31"/>
+      <c r="FT12" s="31"/>
+      <c r="FU12" s="30"/>
+      <c r="FV12" s="30"/>
+      <c r="FW12" s="30"/>
+      <c r="FX12" s="30"/>
+      <c r="FY12" s="30"/>
+      <c r="FZ12" s="146"/>
     </row>
-    <row r="13" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:182" x14ac:dyDescent="0.25">
       <c r="A13" s="123"/>
       <c r="B13" s="29"/>
       <c r="C13" s="30"/>
@@ -13003,8 +13315,38 @@
       <c r="ET13" s="28"/>
       <c r="EU13" s="28"/>
       <c r="EV13" s="33"/>
+      <c r="EW13" s="63"/>
+      <c r="EX13" s="31"/>
+      <c r="EY13" s="31"/>
+      <c r="EZ13" s="30"/>
+      <c r="FA13" s="30"/>
+      <c r="FB13" s="31"/>
+      <c r="FC13" s="30"/>
+      <c r="FD13" s="30"/>
+      <c r="FE13" s="31"/>
+      <c r="FF13" s="31"/>
+      <c r="FG13" s="30"/>
+      <c r="FH13" s="30"/>
+      <c r="FI13" s="31"/>
+      <c r="FJ13" s="30"/>
+      <c r="FK13" s="30"/>
+      <c r="FL13" s="31"/>
+      <c r="FM13" s="31"/>
+      <c r="FN13" s="30"/>
+      <c r="FO13" s="30"/>
+      <c r="FP13" s="30"/>
+      <c r="FQ13" s="30"/>
+      <c r="FR13" s="30"/>
+      <c r="FS13" s="31"/>
+      <c r="FT13" s="31"/>
+      <c r="FU13" s="30"/>
+      <c r="FV13" s="30"/>
+      <c r="FW13" s="30"/>
+      <c r="FX13" s="30"/>
+      <c r="FY13" s="30"/>
+      <c r="FZ13" s="146"/>
     </row>
-    <row r="14" spans="1:152" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:182" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="128"/>
       <c r="B14" s="50"/>
       <c r="C14" s="51"/>
@@ -13157,8 +13499,38 @@
       <c r="ET14" s="53"/>
       <c r="EU14" s="53"/>
       <c r="EV14" s="100"/>
+      <c r="EW14" s="64"/>
+      <c r="EX14" s="52"/>
+      <c r="EY14" s="52"/>
+      <c r="EZ14" s="51"/>
+      <c r="FA14" s="51"/>
+      <c r="FB14" s="52"/>
+      <c r="FC14" s="51"/>
+      <c r="FD14" s="51"/>
+      <c r="FE14" s="52"/>
+      <c r="FF14" s="52"/>
+      <c r="FG14" s="51"/>
+      <c r="FH14" s="51"/>
+      <c r="FI14" s="52"/>
+      <c r="FJ14" s="51"/>
+      <c r="FK14" s="51"/>
+      <c r="FL14" s="52"/>
+      <c r="FM14" s="52"/>
+      <c r="FN14" s="51"/>
+      <c r="FO14" s="51"/>
+      <c r="FP14" s="51"/>
+      <c r="FQ14" s="51"/>
+      <c r="FR14" s="51"/>
+      <c r="FS14" s="52"/>
+      <c r="FT14" s="52"/>
+      <c r="FU14" s="51"/>
+      <c r="FV14" s="51"/>
+      <c r="FW14" s="51"/>
+      <c r="FX14" s="51"/>
+      <c r="FY14" s="51"/>
+      <c r="FZ14" s="147"/>
     </row>
-    <row r="15" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:182" x14ac:dyDescent="0.25">
       <c r="A15" s="125" t="s">
         <v>11</v>
       </c>
@@ -13266,22 +13638,22 @@
       <c r="CS15" s="43"/>
       <c r="CT15" s="44"/>
       <c r="CU15" s="44"/>
-      <c r="CV15" s="45" t="s">
-        <v>58</v>
-      </c>
+      <c r="CV15" s="45"/>
       <c r="CW15" s="43"/>
       <c r="CX15" s="43"/>
       <c r="CY15" s="43"/>
       <c r="CZ15" s="43"/>
       <c r="DA15" s="44"/>
       <c r="DB15" s="44"/>
-      <c r="DC15" s="45"/>
-      <c r="DD15" s="43"/>
-      <c r="DE15" s="43"/>
-      <c r="DF15" s="43"/>
-      <c r="DG15" s="43"/>
-      <c r="DH15" s="44"/>
-      <c r="DI15" s="44"/>
+      <c r="DC15" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="DD15" s="60"/>
+      <c r="DE15" s="60"/>
+      <c r="DF15" s="60"/>
+      <c r="DG15" s="60"/>
+      <c r="DH15" s="60"/>
+      <c r="DI15" s="60"/>
       <c r="DJ15" s="45"/>
       <c r="DK15" s="43"/>
       <c r="DL15" s="43"/>
@@ -13321,8 +13693,38 @@
       <c r="ET15" s="78"/>
       <c r="EU15" s="78"/>
       <c r="EV15" s="102"/>
+      <c r="EW15" s="66"/>
+      <c r="EX15" s="44"/>
+      <c r="EY15" s="44"/>
+      <c r="EZ15" s="43"/>
+      <c r="FA15" s="43"/>
+      <c r="FB15" s="44"/>
+      <c r="FC15" s="43"/>
+      <c r="FD15" s="43"/>
+      <c r="FE15" s="44"/>
+      <c r="FF15" s="44"/>
+      <c r="FG15" s="43"/>
+      <c r="FH15" s="43"/>
+      <c r="FI15" s="44"/>
+      <c r="FJ15" s="43"/>
+      <c r="FK15" s="43"/>
+      <c r="FL15" s="44"/>
+      <c r="FM15" s="44"/>
+      <c r="FN15" s="43"/>
+      <c r="FO15" s="43"/>
+      <c r="FP15" s="43"/>
+      <c r="FQ15" s="43"/>
+      <c r="FR15" s="43"/>
+      <c r="FS15" s="44"/>
+      <c r="FT15" s="44"/>
+      <c r="FU15" s="43"/>
+      <c r="FV15" s="43"/>
+      <c r="FW15" s="43"/>
+      <c r="FX15" s="43"/>
+      <c r="FY15" s="43"/>
+      <c r="FZ15" s="148"/>
     </row>
-    <row r="16" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:182" x14ac:dyDescent="0.25">
       <c r="A16" s="123"/>
       <c r="B16" s="24"/>
       <c r="C16" s="16"/>
@@ -13394,7 +13796,7 @@
       <c r="BO16" s="113"/>
       <c r="BP16" s="113"/>
       <c r="BQ16" s="56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="BR16" s="14"/>
       <c r="BS16" s="14"/>
@@ -13481,8 +13883,38 @@
       <c r="ET16" s="13"/>
       <c r="EU16" s="13"/>
       <c r="EV16" s="17"/>
+      <c r="EW16" s="67"/>
+      <c r="EX16" s="140"/>
+      <c r="EY16" s="14"/>
+      <c r="EZ16" s="16"/>
+      <c r="FA16" s="16"/>
+      <c r="FB16" s="14"/>
+      <c r="FC16" s="16"/>
+      <c r="FD16" s="16"/>
+      <c r="FE16" s="14"/>
+      <c r="FF16" s="14"/>
+      <c r="FG16" s="16"/>
+      <c r="FH16" s="16"/>
+      <c r="FI16" s="14"/>
+      <c r="FJ16" s="16"/>
+      <c r="FK16" s="16"/>
+      <c r="FL16" s="14"/>
+      <c r="FM16" s="14"/>
+      <c r="FN16" s="16"/>
+      <c r="FO16" s="16"/>
+      <c r="FP16" s="16"/>
+      <c r="FQ16" s="16"/>
+      <c r="FR16" s="16"/>
+      <c r="FS16" s="14"/>
+      <c r="FT16" s="14"/>
+      <c r="FU16" s="16"/>
+      <c r="FV16" s="16"/>
+      <c r="FW16" s="16"/>
+      <c r="FX16" s="16"/>
+      <c r="FY16" s="16"/>
+      <c r="FZ16" s="149"/>
     </row>
-    <row r="17" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:182" x14ac:dyDescent="0.25">
       <c r="A17" s="123"/>
       <c r="B17" s="24"/>
       <c r="C17" s="16"/>
@@ -13639,8 +14071,38 @@
       <c r="ET17" s="13"/>
       <c r="EU17" s="13"/>
       <c r="EV17" s="17"/>
+      <c r="EW17" s="67"/>
+      <c r="EX17" s="14"/>
+      <c r="EY17" s="14"/>
+      <c r="EZ17" s="16"/>
+      <c r="FA17" s="16"/>
+      <c r="FB17" s="14"/>
+      <c r="FC17" s="16"/>
+      <c r="FD17" s="16"/>
+      <c r="FE17" s="14"/>
+      <c r="FF17" s="14"/>
+      <c r="FG17" s="16"/>
+      <c r="FH17" s="16"/>
+      <c r="FI17" s="14"/>
+      <c r="FJ17" s="16"/>
+      <c r="FK17" s="16"/>
+      <c r="FL17" s="14"/>
+      <c r="FM17" s="14"/>
+      <c r="FN17" s="16"/>
+      <c r="FO17" s="16"/>
+      <c r="FP17" s="16"/>
+      <c r="FQ17" s="16"/>
+      <c r="FR17" s="16"/>
+      <c r="FS17" s="14"/>
+      <c r="FT17" s="14"/>
+      <c r="FU17" s="16"/>
+      <c r="FV17" s="16"/>
+      <c r="FW17" s="16"/>
+      <c r="FX17" s="16"/>
+      <c r="FY17" s="16"/>
+      <c r="FZ17" s="149"/>
     </row>
-    <row r="18" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:182" x14ac:dyDescent="0.25">
       <c r="A18" s="123"/>
       <c r="B18" s="24"/>
       <c r="C18" s="16"/>
@@ -13744,13 +14206,13 @@
       <c r="CU18" s="14"/>
       <c r="CV18" s="13"/>
       <c r="CW18" s="16"/>
-      <c r="CX18" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="CY18" s="16"/>
-      <c r="CZ18" s="16"/>
-      <c r="DA18" s="14"/>
-      <c r="DB18" s="14"/>
+      <c r="CX18" s="59" t="s">
+        <v>66</v>
+      </c>
+      <c r="CY18" s="59"/>
+      <c r="CZ18" s="59"/>
+      <c r="DA18" s="59"/>
+      <c r="DB18" s="59"/>
       <c r="DC18" s="13"/>
       <c r="DD18" s="16"/>
       <c r="DE18" s="16"/>
@@ -13797,8 +14259,38 @@
       <c r="ET18" s="13"/>
       <c r="EU18" s="13"/>
       <c r="EV18" s="17"/>
+      <c r="EW18" s="67"/>
+      <c r="EX18" s="140"/>
+      <c r="EY18" s="14"/>
+      <c r="EZ18" s="16"/>
+      <c r="FA18" s="16"/>
+      <c r="FB18" s="14"/>
+      <c r="FC18" s="16"/>
+      <c r="FD18" s="16"/>
+      <c r="FE18" s="14"/>
+      <c r="FF18" s="14"/>
+      <c r="FG18" s="16"/>
+      <c r="FH18" s="16"/>
+      <c r="FI18" s="14"/>
+      <c r="FJ18" s="16"/>
+      <c r="FK18" s="16"/>
+      <c r="FL18" s="14"/>
+      <c r="FM18" s="14"/>
+      <c r="FN18" s="16"/>
+      <c r="FO18" s="16"/>
+      <c r="FP18" s="16"/>
+      <c r="FQ18" s="16"/>
+      <c r="FR18" s="16"/>
+      <c r="FS18" s="14"/>
+      <c r="FT18" s="14"/>
+      <c r="FU18" s="16"/>
+      <c r="FV18" s="16"/>
+      <c r="FW18" s="16"/>
+      <c r="FX18" s="16"/>
+      <c r="FY18" s="16"/>
+      <c r="FZ18" s="149"/>
     </row>
-    <row r="19" spans="1:152" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:182" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="123"/>
       <c r="B19" s="26"/>
       <c r="C19" s="21"/>
@@ -13901,7 +14393,7 @@
       <c r="CV19" s="16"/>
       <c r="CW19" s="21"/>
       <c r="CX19" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="CY19" s="21"/>
       <c r="CZ19" s="21"/>
@@ -13953,8 +14445,38 @@
       <c r="ET19" s="73"/>
       <c r="EU19" s="73"/>
       <c r="EV19" s="98"/>
+      <c r="EW19" s="68"/>
+      <c r="EX19" s="20"/>
+      <c r="EY19" s="20"/>
+      <c r="EZ19" s="21"/>
+      <c r="FA19" s="21"/>
+      <c r="FB19" s="20"/>
+      <c r="FC19" s="21"/>
+      <c r="FD19" s="21"/>
+      <c r="FE19" s="14"/>
+      <c r="FF19" s="20"/>
+      <c r="FG19" s="16"/>
+      <c r="FH19" s="21"/>
+      <c r="FI19" s="20"/>
+      <c r="FJ19" s="21"/>
+      <c r="FK19" s="21"/>
+      <c r="FL19" s="20"/>
+      <c r="FM19" s="20"/>
+      <c r="FN19" s="21"/>
+      <c r="FO19" s="21"/>
+      <c r="FP19" s="21"/>
+      <c r="FQ19" s="21"/>
+      <c r="FR19" s="21"/>
+      <c r="FS19" s="20"/>
+      <c r="FT19" s="20"/>
+      <c r="FU19" s="21"/>
+      <c r="FV19" s="21"/>
+      <c r="FW19" s="21"/>
+      <c r="FX19" s="21"/>
+      <c r="FY19" s="21"/>
+      <c r="FZ19" s="150"/>
     </row>
-    <row r="20" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="125" t="s">
         <v>17</v>
       </c>
@@ -14117,8 +14639,38 @@
       <c r="ET20" s="78"/>
       <c r="EU20" s="78"/>
       <c r="EV20" s="102"/>
+      <c r="EW20" s="82"/>
+      <c r="EX20" s="77"/>
+      <c r="EY20" s="77"/>
+      <c r="EZ20" s="86"/>
+      <c r="FA20" s="76"/>
+      <c r="FB20" s="77"/>
+      <c r="FC20" s="76"/>
+      <c r="FD20" s="76"/>
+      <c r="FE20" s="77"/>
+      <c r="FF20" s="77"/>
+      <c r="FG20" s="86"/>
+      <c r="FH20" s="76"/>
+      <c r="FI20" s="77"/>
+      <c r="FJ20" s="76"/>
+      <c r="FK20" s="76"/>
+      <c r="FL20" s="77"/>
+      <c r="FM20" s="77"/>
+      <c r="FN20" s="86"/>
+      <c r="FO20" s="76"/>
+      <c r="FP20" s="76"/>
+      <c r="FQ20" s="76"/>
+      <c r="FR20" s="76"/>
+      <c r="FS20" s="77"/>
+      <c r="FT20" s="77"/>
+      <c r="FU20" s="86"/>
+      <c r="FV20" s="76"/>
+      <c r="FW20" s="76"/>
+      <c r="FX20" s="76"/>
+      <c r="FY20" s="76"/>
+      <c r="FZ20" s="151"/>
     </row>
-    <row r="21" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="123"/>
       <c r="B21" s="24"/>
       <c r="C21" s="16"/>
@@ -14202,7 +14754,7 @@
       <c r="BY21" s="14"/>
       <c r="BZ21" s="14"/>
       <c r="CA21" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="CB21" s="16"/>
       <c r="CC21" s="16"/>
@@ -14217,9 +14769,7 @@
       <c r="CL21" s="16"/>
       <c r="CM21" s="14"/>
       <c r="CN21" s="24"/>
-      <c r="CO21" s="23" t="s">
-        <v>53</v>
-      </c>
+      <c r="CO21" s="23"/>
       <c r="CP21" s="16"/>
       <c r="CQ21" s="16"/>
       <c r="CR21" s="16"/>
@@ -14279,8 +14829,38 @@
       <c r="ET21" s="13"/>
       <c r="EU21" s="13"/>
       <c r="EV21" s="17"/>
+      <c r="EW21" s="67"/>
+      <c r="EX21" s="140"/>
+      <c r="EY21" s="14"/>
+      <c r="EZ21" s="16"/>
+      <c r="FA21" s="16"/>
+      <c r="FB21" s="14"/>
+      <c r="FC21" s="16"/>
+      <c r="FD21" s="16"/>
+      <c r="FE21" s="14"/>
+      <c r="FF21" s="14"/>
+      <c r="FG21" s="16"/>
+      <c r="FH21" s="16"/>
+      <c r="FI21" s="14"/>
+      <c r="FJ21" s="16"/>
+      <c r="FK21" s="16"/>
+      <c r="FL21" s="14"/>
+      <c r="FM21" s="14"/>
+      <c r="FN21" s="16"/>
+      <c r="FO21" s="16"/>
+      <c r="FP21" s="16"/>
+      <c r="FQ21" s="16"/>
+      <c r="FR21" s="16"/>
+      <c r="FS21" s="14"/>
+      <c r="FT21" s="14"/>
+      <c r="FU21" s="16"/>
+      <c r="FV21" s="16"/>
+      <c r="FW21" s="16"/>
+      <c r="FX21" s="16"/>
+      <c r="FY21" s="16"/>
+      <c r="FZ21" s="149"/>
     </row>
-    <row r="22" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="123"/>
       <c r="B22" s="24"/>
       <c r="C22" s="16"/>
@@ -14437,8 +15017,38 @@
       <c r="ET22" s="13"/>
       <c r="EU22" s="13"/>
       <c r="EV22" s="17"/>
+      <c r="EW22" s="67"/>
+      <c r="EX22" s="14"/>
+      <c r="EY22" s="14"/>
+      <c r="EZ22" s="16"/>
+      <c r="FA22" s="16"/>
+      <c r="FB22" s="14"/>
+      <c r="FC22" s="16"/>
+      <c r="FD22" s="16"/>
+      <c r="FE22" s="14"/>
+      <c r="FF22" s="14"/>
+      <c r="FG22" s="16"/>
+      <c r="FH22" s="16"/>
+      <c r="FI22" s="14"/>
+      <c r="FJ22" s="16"/>
+      <c r="FK22" s="16"/>
+      <c r="FL22" s="14"/>
+      <c r="FM22" s="14"/>
+      <c r="FN22" s="16"/>
+      <c r="FO22" s="16"/>
+      <c r="FP22" s="16"/>
+      <c r="FQ22" s="16"/>
+      <c r="FR22" s="16"/>
+      <c r="FS22" s="14"/>
+      <c r="FT22" s="14"/>
+      <c r="FU22" s="16"/>
+      <c r="FV22" s="16"/>
+      <c r="FW22" s="16"/>
+      <c r="FX22" s="16"/>
+      <c r="FY22" s="16"/>
+      <c r="FZ22" s="149"/>
     </row>
-    <row r="23" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="123"/>
       <c r="B23" s="24"/>
       <c r="C23" s="13"/>
@@ -14535,7 +15145,9 @@
       <c r="CL23" s="13"/>
       <c r="CM23" s="14"/>
       <c r="CN23" s="24"/>
-      <c r="CO23" s="13"/>
+      <c r="CO23" s="23" t="s">
+        <v>53</v>
+      </c>
       <c r="CP23" s="13"/>
       <c r="CQ23" s="13"/>
       <c r="CR23" s="13"/>
@@ -14544,11 +15156,13 @@
       <c r="CU23" s="14"/>
       <c r="CV23" s="13"/>
       <c r="CW23" s="13"/>
-      <c r="CX23" s="13"/>
-      <c r="CY23" s="13"/>
-      <c r="CZ23" s="13"/>
-      <c r="DA23" s="14"/>
-      <c r="DB23" s="14"/>
+      <c r="CX23" s="59" t="s">
+        <v>66</v>
+      </c>
+      <c r="CY23" s="59"/>
+      <c r="CZ23" s="59"/>
+      <c r="DA23" s="59"/>
+      <c r="DB23" s="59"/>
       <c r="DC23" s="13"/>
       <c r="DD23" s="13"/>
       <c r="DE23" s="13"/>
@@ -14595,8 +15209,38 @@
       <c r="ET23" s="13"/>
       <c r="EU23" s="13"/>
       <c r="EV23" s="17"/>
+      <c r="EW23" s="67"/>
+      <c r="EX23" s="140"/>
+      <c r="EY23" s="14"/>
+      <c r="EZ23" s="16"/>
+      <c r="FA23" s="16"/>
+      <c r="FB23" s="14"/>
+      <c r="FC23" s="16"/>
+      <c r="FD23" s="16"/>
+      <c r="FE23" s="14"/>
+      <c r="FF23" s="14"/>
+      <c r="FG23" s="16"/>
+      <c r="FH23" s="16"/>
+      <c r="FI23" s="14"/>
+      <c r="FJ23" s="16"/>
+      <c r="FK23" s="16"/>
+      <c r="FL23" s="14"/>
+      <c r="FM23" s="14"/>
+      <c r="FN23" s="16"/>
+      <c r="FO23" s="16"/>
+      <c r="FP23" s="16"/>
+      <c r="FQ23" s="16"/>
+      <c r="FR23" s="16"/>
+      <c r="FS23" s="14"/>
+      <c r="FT23" s="14"/>
+      <c r="FU23" s="16"/>
+      <c r="FV23" s="16"/>
+      <c r="FW23" s="16"/>
+      <c r="FX23" s="16"/>
+      <c r="FY23" s="16"/>
+      <c r="FZ23" s="149"/>
     </row>
-    <row r="24" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:182" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="124"/>
       <c r="B24" s="91"/>
       <c r="C24" s="92"/>
@@ -14749,8 +15393,38 @@
       <c r="ET24" s="73"/>
       <c r="EU24" s="73"/>
       <c r="EV24" s="98"/>
+      <c r="EW24" s="138"/>
+      <c r="EX24" s="93"/>
+      <c r="EY24" s="93"/>
+      <c r="EZ24" s="139"/>
+      <c r="FA24" s="139"/>
+      <c r="FB24" s="93"/>
+      <c r="FC24" s="139"/>
+      <c r="FD24" s="139"/>
+      <c r="FE24" s="93"/>
+      <c r="FF24" s="93"/>
+      <c r="FG24" s="139"/>
+      <c r="FH24" s="139"/>
+      <c r="FI24" s="93"/>
+      <c r="FJ24" s="139"/>
+      <c r="FK24" s="139"/>
+      <c r="FL24" s="93"/>
+      <c r="FM24" s="93"/>
+      <c r="FN24" s="139"/>
+      <c r="FO24" s="139"/>
+      <c r="FP24" s="139"/>
+      <c r="FQ24" s="139"/>
+      <c r="FR24" s="139"/>
+      <c r="FS24" s="93"/>
+      <c r="FT24" s="93"/>
+      <c r="FU24" s="139"/>
+      <c r="FV24" s="139"/>
+      <c r="FW24" s="139"/>
+      <c r="FX24" s="139"/>
+      <c r="FY24" s="139"/>
+      <c r="FZ24" s="152"/>
     </row>
-    <row r="25" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="125" t="s">
         <v>25</v>
       </c>
@@ -14905,8 +15579,38 @@
       <c r="ET25" s="78"/>
       <c r="EU25" s="78"/>
       <c r="EV25" s="102"/>
+      <c r="EW25" s="82"/>
+      <c r="EX25" s="77"/>
+      <c r="EY25" s="77"/>
+      <c r="EZ25" s="76"/>
+      <c r="FA25" s="76"/>
+      <c r="FB25" s="77"/>
+      <c r="FC25" s="76"/>
+      <c r="FD25" s="76"/>
+      <c r="FE25" s="77"/>
+      <c r="FF25" s="77"/>
+      <c r="FG25" s="76"/>
+      <c r="FH25" s="76"/>
+      <c r="FI25" s="77"/>
+      <c r="FJ25" s="76"/>
+      <c r="FK25" s="76"/>
+      <c r="FL25" s="77"/>
+      <c r="FM25" s="77"/>
+      <c r="FN25" s="76"/>
+      <c r="FO25" s="76"/>
+      <c r="FP25" s="76"/>
+      <c r="FQ25" s="76"/>
+      <c r="FR25" s="76"/>
+      <c r="FS25" s="77"/>
+      <c r="FT25" s="77"/>
+      <c r="FU25" s="76"/>
+      <c r="FV25" s="76"/>
+      <c r="FW25" s="76"/>
+      <c r="FX25" s="76"/>
+      <c r="FY25" s="76"/>
+      <c r="FZ25" s="151"/>
     </row>
-    <row r="26" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="123"/>
       <c r="B26" s="24"/>
       <c r="C26" s="16"/>
@@ -15059,8 +15763,38 @@
       <c r="ET26" s="13"/>
       <c r="EU26" s="13"/>
       <c r="EV26" s="17"/>
+      <c r="EW26" s="67"/>
+      <c r="EX26" s="14"/>
+      <c r="EY26" s="14"/>
+      <c r="EZ26" s="16"/>
+      <c r="FA26" s="16"/>
+      <c r="FB26" s="14"/>
+      <c r="FC26" s="16"/>
+      <c r="FD26" s="16"/>
+      <c r="FE26" s="14"/>
+      <c r="FF26" s="14"/>
+      <c r="FG26" s="16"/>
+      <c r="FH26" s="16"/>
+      <c r="FI26" s="14"/>
+      <c r="FJ26" s="16"/>
+      <c r="FK26" s="16"/>
+      <c r="FL26" s="14"/>
+      <c r="FM26" s="14"/>
+      <c r="FN26" s="16"/>
+      <c r="FO26" s="16"/>
+      <c r="FP26" s="16"/>
+      <c r="FQ26" s="16"/>
+      <c r="FR26" s="16"/>
+      <c r="FS26" s="14"/>
+      <c r="FT26" s="14"/>
+      <c r="FU26" s="16"/>
+      <c r="FV26" s="16"/>
+      <c r="FW26" s="16"/>
+      <c r="FX26" s="16"/>
+      <c r="FY26" s="16"/>
+      <c r="FZ26" s="149"/>
     </row>
-    <row r="27" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="123"/>
       <c r="B27" s="24"/>
       <c r="C27" s="16"/>
@@ -15213,8 +15947,38 @@
       <c r="ET27" s="13"/>
       <c r="EU27" s="13"/>
       <c r="EV27" s="17"/>
+      <c r="EW27" s="67"/>
+      <c r="EX27" s="14"/>
+      <c r="EY27" s="14"/>
+      <c r="EZ27" s="16"/>
+      <c r="FA27" s="16"/>
+      <c r="FB27" s="14"/>
+      <c r="FC27" s="16"/>
+      <c r="FD27" s="16"/>
+      <c r="FE27" s="14"/>
+      <c r="FF27" s="14"/>
+      <c r="FG27" s="16"/>
+      <c r="FH27" s="16"/>
+      <c r="FI27" s="14"/>
+      <c r="FJ27" s="16"/>
+      <c r="FK27" s="16"/>
+      <c r="FL27" s="14"/>
+      <c r="FM27" s="14"/>
+      <c r="FN27" s="16"/>
+      <c r="FO27" s="16"/>
+      <c r="FP27" s="16"/>
+      <c r="FQ27" s="16"/>
+      <c r="FR27" s="16"/>
+      <c r="FS27" s="14"/>
+      <c r="FT27" s="14"/>
+      <c r="FU27" s="16"/>
+      <c r="FV27" s="16"/>
+      <c r="FW27" s="16"/>
+      <c r="FX27" s="16"/>
+      <c r="FY27" s="16"/>
+      <c r="FZ27" s="149"/>
     </row>
-    <row r="28" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="123"/>
       <c r="B28" s="24"/>
       <c r="C28" s="16"/>
@@ -15367,8 +16131,38 @@
       <c r="ET28" s="13"/>
       <c r="EU28" s="13"/>
       <c r="EV28" s="17"/>
+      <c r="EW28" s="67"/>
+      <c r="EX28" s="14"/>
+      <c r="EY28" s="14"/>
+      <c r="EZ28" s="16"/>
+      <c r="FA28" s="16"/>
+      <c r="FB28" s="14"/>
+      <c r="FC28" s="16"/>
+      <c r="FD28" s="16"/>
+      <c r="FE28" s="14"/>
+      <c r="FF28" s="14"/>
+      <c r="FG28" s="16"/>
+      <c r="FH28" s="16"/>
+      <c r="FI28" s="14"/>
+      <c r="FJ28" s="16"/>
+      <c r="FK28" s="16"/>
+      <c r="FL28" s="14"/>
+      <c r="FM28" s="14"/>
+      <c r="FN28" s="16"/>
+      <c r="FO28" s="16"/>
+      <c r="FP28" s="16"/>
+      <c r="FQ28" s="16"/>
+      <c r="FR28" s="16"/>
+      <c r="FS28" s="14"/>
+      <c r="FT28" s="14"/>
+      <c r="FU28" s="16"/>
+      <c r="FV28" s="16"/>
+      <c r="FW28" s="16"/>
+      <c r="FX28" s="16"/>
+      <c r="FY28" s="16"/>
+      <c r="FZ28" s="149"/>
     </row>
-    <row r="29" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:182" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="123"/>
       <c r="B29" s="85"/>
       <c r="C29" s="71"/>
@@ -15521,8 +16315,38 @@
       <c r="ET29" s="73"/>
       <c r="EU29" s="73"/>
       <c r="EV29" s="98"/>
+      <c r="EW29" s="70"/>
+      <c r="EX29" s="72"/>
+      <c r="EY29" s="72"/>
+      <c r="EZ29" s="71"/>
+      <c r="FA29" s="71"/>
+      <c r="FB29" s="72"/>
+      <c r="FC29" s="71"/>
+      <c r="FD29" s="71"/>
+      <c r="FE29" s="72"/>
+      <c r="FF29" s="72"/>
+      <c r="FG29" s="71"/>
+      <c r="FH29" s="71"/>
+      <c r="FI29" s="72"/>
+      <c r="FJ29" s="71"/>
+      <c r="FK29" s="71"/>
+      <c r="FL29" s="72"/>
+      <c r="FM29" s="72"/>
+      <c r="FN29" s="71"/>
+      <c r="FO29" s="71"/>
+      <c r="FP29" s="71"/>
+      <c r="FQ29" s="71"/>
+      <c r="FR29" s="71"/>
+      <c r="FS29" s="72"/>
+      <c r="FT29" s="72"/>
+      <c r="FU29" s="71"/>
+      <c r="FV29" s="71"/>
+      <c r="FW29" s="71"/>
+      <c r="FX29" s="71"/>
+      <c r="FY29" s="71"/>
+      <c r="FZ29" s="152"/>
     </row>
-    <row r="30" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="122" t="s">
         <v>20</v>
       </c>
@@ -15632,10 +16456,10 @@
       <c r="CS30" s="76"/>
       <c r="CT30" s="77"/>
       <c r="CU30" s="77"/>
-      <c r="CV30" s="78" t="s">
-        <v>60</v>
-      </c>
-      <c r="CW30" s="76"/>
+      <c r="CV30" s="88" t="s">
+        <v>59</v>
+      </c>
+      <c r="CW30" s="88"/>
       <c r="CX30" s="76"/>
       <c r="CY30" s="76"/>
       <c r="CZ30" s="76"/>
@@ -15651,13 +16475,15 @@
       <c r="DJ30" s="78"/>
       <c r="DK30" s="76"/>
       <c r="DL30" s="76"/>
-      <c r="DM30" s="76"/>
-      <c r="DN30" s="76"/>
-      <c r="DO30" s="77"/>
-      <c r="DP30" s="77"/>
-      <c r="DQ30" s="84"/>
-      <c r="DR30" s="82"/>
-      <c r="DS30" s="76"/>
+      <c r="DM30" s="88" t="s">
+        <v>2</v>
+      </c>
+      <c r="DN30" s="88"/>
+      <c r="DO30" s="88"/>
+      <c r="DP30" s="88"/>
+      <c r="DQ30" s="135"/>
+      <c r="DR30" s="136"/>
+      <c r="DS30" s="88"/>
       <c r="DT30" s="76"/>
       <c r="DU30" s="76"/>
       <c r="DV30" s="77"/>
@@ -15687,8 +16513,38 @@
       <c r="ET30" s="78"/>
       <c r="EU30" s="78"/>
       <c r="EV30" s="102"/>
+      <c r="EW30" s="82"/>
+      <c r="EX30" s="77"/>
+      <c r="EY30" s="77"/>
+      <c r="EZ30" s="76"/>
+      <c r="FA30" s="76"/>
+      <c r="FB30" s="77"/>
+      <c r="FC30" s="76"/>
+      <c r="FD30" s="76"/>
+      <c r="FE30" s="77"/>
+      <c r="FF30" s="77"/>
+      <c r="FG30" s="76"/>
+      <c r="FH30" s="76"/>
+      <c r="FI30" s="77"/>
+      <c r="FJ30" s="76"/>
+      <c r="FK30" s="76"/>
+      <c r="FL30" s="77"/>
+      <c r="FM30" s="77"/>
+      <c r="FN30" s="76"/>
+      <c r="FO30" s="76"/>
+      <c r="FP30" s="76"/>
+      <c r="FQ30" s="76"/>
+      <c r="FR30" s="76"/>
+      <c r="FS30" s="77"/>
+      <c r="FT30" s="77"/>
+      <c r="FU30" s="76"/>
+      <c r="FV30" s="76"/>
+      <c r="FW30" s="76"/>
+      <c r="FX30" s="76"/>
+      <c r="FY30" s="76"/>
+      <c r="FZ30" s="151"/>
     </row>
-    <row r="31" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="123"/>
       <c r="B31" s="24"/>
       <c r="C31" s="16"/>
@@ -15790,10 +16646,10 @@
       <c r="CS31" s="16"/>
       <c r="CT31" s="14"/>
       <c r="CU31" s="14"/>
-      <c r="CV31" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="CW31" s="16"/>
+      <c r="CV31" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="CW31" s="59"/>
       <c r="CX31" s="16"/>
       <c r="CY31" s="16"/>
       <c r="CZ31" s="16"/>
@@ -15845,8 +16701,38 @@
       <c r="ET31" s="13"/>
       <c r="EU31" s="13"/>
       <c r="EV31" s="17"/>
+      <c r="EW31" s="67"/>
+      <c r="EX31" s="14"/>
+      <c r="EY31" s="14"/>
+      <c r="EZ31" s="16"/>
+      <c r="FA31" s="16"/>
+      <c r="FB31" s="14"/>
+      <c r="FC31" s="16"/>
+      <c r="FD31" s="16"/>
+      <c r="FE31" s="14"/>
+      <c r="FF31" s="14"/>
+      <c r="FG31" s="16"/>
+      <c r="FH31" s="16"/>
+      <c r="FI31" s="14"/>
+      <c r="FJ31" s="16"/>
+      <c r="FK31" s="16"/>
+      <c r="FL31" s="140"/>
+      <c r="FM31" s="14"/>
+      <c r="FN31" s="16"/>
+      <c r="FO31" s="16"/>
+      <c r="FP31" s="16"/>
+      <c r="FQ31" s="16"/>
+      <c r="FR31" s="16"/>
+      <c r="FS31" s="14"/>
+      <c r="FT31" s="14"/>
+      <c r="FU31" s="16"/>
+      <c r="FV31" s="16"/>
+      <c r="FW31" s="16"/>
+      <c r="FX31" s="16"/>
+      <c r="FY31" s="16"/>
+      <c r="FZ31" s="149"/>
     </row>
-    <row r="32" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="123"/>
       <c r="B32" s="24"/>
       <c r="C32" s="16"/>
@@ -15921,7 +16807,7 @@
       <c r="BT32" s="16"/>
       <c r="BU32" s="16"/>
       <c r="BV32" s="56" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="BW32" s="16"/>
       <c r="BX32" s="16"/>
@@ -15952,7 +16838,7 @@
       <c r="CU32" s="14"/>
       <c r="CV32" s="16"/>
       <c r="CW32" s="16"/>
-      <c r="CX32" s="16" t="s">
+      <c r="CX32" s="59" t="s">
         <v>54</v>
       </c>
       <c r="CY32" s="16"/>
@@ -15966,11 +16852,11 @@
       <c r="DG32" s="16"/>
       <c r="DH32" s="14"/>
       <c r="DI32" s="14"/>
-      <c r="DJ32" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="DK32" s="16"/>
-      <c r="DL32" s="16"/>
+      <c r="DJ32" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="DK32" s="59"/>
+      <c r="DL32" s="59"/>
       <c r="DM32" s="16"/>
       <c r="DN32" s="16"/>
       <c r="DO32" s="14"/>
@@ -16007,8 +16893,38 @@
       <c r="ET32" s="13"/>
       <c r="EU32" s="13"/>
       <c r="EV32" s="17"/>
+      <c r="EW32" s="67"/>
+      <c r="EX32" s="14"/>
+      <c r="EY32" s="14"/>
+      <c r="EZ32" s="16"/>
+      <c r="FA32" s="16"/>
+      <c r="FB32" s="14"/>
+      <c r="FC32" s="16"/>
+      <c r="FD32" s="16"/>
+      <c r="FE32" s="14"/>
+      <c r="FF32" s="14"/>
+      <c r="FG32" s="16"/>
+      <c r="FH32" s="16"/>
+      <c r="FI32" s="14"/>
+      <c r="FJ32" s="16"/>
+      <c r="FK32" s="16"/>
+      <c r="FL32" s="14"/>
+      <c r="FM32" s="14"/>
+      <c r="FN32" s="16"/>
+      <c r="FO32" s="16"/>
+      <c r="FP32" s="16"/>
+      <c r="FQ32" s="16"/>
+      <c r="FR32" s="16"/>
+      <c r="FS32" s="14"/>
+      <c r="FT32" s="14"/>
+      <c r="FU32" s="16"/>
+      <c r="FV32" s="16"/>
+      <c r="FW32" s="16"/>
+      <c r="FX32" s="16"/>
+      <c r="FY32" s="16"/>
+      <c r="FZ32" s="149"/>
     </row>
-    <row r="33" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="123"/>
       <c r="B33" s="24"/>
       <c r="C33" s="16"/>
@@ -16110,7 +17026,7 @@
       <c r="CU33" s="14"/>
       <c r="CV33" s="23"/>
       <c r="CW33" s="16"/>
-      <c r="CX33" s="23" t="s">
+      <c r="CX33" s="133" t="s">
         <v>53</v>
       </c>
       <c r="CY33" s="16"/>
@@ -16163,8 +17079,38 @@
       <c r="ET33" s="13"/>
       <c r="EU33" s="13"/>
       <c r="EV33" s="17"/>
+      <c r="EW33" s="67"/>
+      <c r="EX33" s="14"/>
+      <c r="EY33" s="14"/>
+      <c r="EZ33" s="23"/>
+      <c r="FA33" s="16"/>
+      <c r="FB33" s="14"/>
+      <c r="FC33" s="16"/>
+      <c r="FD33" s="16"/>
+      <c r="FE33" s="140"/>
+      <c r="FF33" s="14"/>
+      <c r="FG33" s="23"/>
+      <c r="FH33" s="16"/>
+      <c r="FI33" s="14"/>
+      <c r="FJ33" s="16"/>
+      <c r="FK33" s="16"/>
+      <c r="FL33" s="14"/>
+      <c r="FM33" s="14"/>
+      <c r="FN33" s="16"/>
+      <c r="FO33" s="16"/>
+      <c r="FP33" s="16"/>
+      <c r="FQ33" s="16"/>
+      <c r="FR33" s="16"/>
+      <c r="FS33" s="14"/>
+      <c r="FT33" s="14"/>
+      <c r="FU33" s="16"/>
+      <c r="FV33" s="16"/>
+      <c r="FW33" s="16"/>
+      <c r="FX33" s="16"/>
+      <c r="FY33" s="16"/>
+      <c r="FZ33" s="149"/>
     </row>
-    <row r="34" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:182" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="124"/>
       <c r="B34" s="85"/>
       <c r="C34" s="71"/>
@@ -16278,7 +17224,9 @@
       <c r="DG34" s="71"/>
       <c r="DH34" s="72"/>
       <c r="DI34" s="72"/>
-      <c r="DJ34" s="73"/>
+      <c r="DJ34" s="16" t="s">
+        <v>64</v>
+      </c>
       <c r="DK34" s="71"/>
       <c r="DL34" s="71"/>
       <c r="DM34" s="71"/>
@@ -16317,8 +17265,38 @@
       <c r="ET34" s="73"/>
       <c r="EU34" s="73"/>
       <c r="EV34" s="98"/>
+      <c r="EW34" s="70"/>
+      <c r="EX34" s="72"/>
+      <c r="EY34" s="72"/>
+      <c r="EZ34" s="71"/>
+      <c r="FA34" s="71"/>
+      <c r="FB34" s="72"/>
+      <c r="FC34" s="71"/>
+      <c r="FD34" s="71"/>
+      <c r="FE34" s="72"/>
+      <c r="FF34" s="72"/>
+      <c r="FG34" s="71"/>
+      <c r="FH34" s="71"/>
+      <c r="FI34" s="72"/>
+      <c r="FJ34" s="71"/>
+      <c r="FK34" s="71"/>
+      <c r="FL34" s="72"/>
+      <c r="FM34" s="72"/>
+      <c r="FN34" s="71"/>
+      <c r="FO34" s="71"/>
+      <c r="FP34" s="71"/>
+      <c r="FQ34" s="71"/>
+      <c r="FR34" s="71"/>
+      <c r="FS34" s="14"/>
+      <c r="FT34" s="72"/>
+      <c r="FU34" s="71"/>
+      <c r="FV34" s="71"/>
+      <c r="FW34" s="71"/>
+      <c r="FX34" s="71"/>
+      <c r="FY34" s="71"/>
+      <c r="FZ34" s="152"/>
     </row>
-    <row r="35" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="123" t="s">
         <v>23</v>
       </c>
@@ -16477,8 +17455,38 @@
       <c r="ET35" s="78"/>
       <c r="EU35" s="78"/>
       <c r="EV35" s="102"/>
+      <c r="EW35" s="82"/>
+      <c r="EX35" s="141"/>
+      <c r="EY35" s="77"/>
+      <c r="EZ35" s="76"/>
+      <c r="FA35" s="76"/>
+      <c r="FB35" s="77"/>
+      <c r="FC35" s="76"/>
+      <c r="FD35" s="76"/>
+      <c r="FE35" s="77"/>
+      <c r="FF35" s="77"/>
+      <c r="FG35" s="76"/>
+      <c r="FH35" s="76"/>
+      <c r="FI35" s="77"/>
+      <c r="FJ35" s="76"/>
+      <c r="FK35" s="76"/>
+      <c r="FL35" s="77"/>
+      <c r="FM35" s="77"/>
+      <c r="FN35" s="76"/>
+      <c r="FO35" s="76"/>
+      <c r="FP35" s="76"/>
+      <c r="FQ35" s="76"/>
+      <c r="FR35" s="76"/>
+      <c r="FS35" s="77"/>
+      <c r="FT35" s="77"/>
+      <c r="FU35" s="76"/>
+      <c r="FV35" s="76"/>
+      <c r="FW35" s="76"/>
+      <c r="FX35" s="76"/>
+      <c r="FY35" s="76"/>
+      <c r="FZ35" s="151"/>
     </row>
-    <row r="36" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="123"/>
       <c r="B36" s="24"/>
       <c r="C36" s="16"/>
@@ -16633,8 +17641,38 @@
       <c r="ET36" s="13"/>
       <c r="EU36" s="13"/>
       <c r="EV36" s="17"/>
+      <c r="EW36" s="67"/>
+      <c r="EX36" s="14"/>
+      <c r="EY36" s="14"/>
+      <c r="EZ36" s="16"/>
+      <c r="FA36" s="16"/>
+      <c r="FB36" s="14"/>
+      <c r="FC36" s="16"/>
+      <c r="FD36" s="16"/>
+      <c r="FE36" s="14"/>
+      <c r="FF36" s="14"/>
+      <c r="FG36" s="16"/>
+      <c r="FH36" s="16"/>
+      <c r="FI36" s="14"/>
+      <c r="FJ36" s="16"/>
+      <c r="FK36" s="16"/>
+      <c r="FL36" s="14"/>
+      <c r="FM36" s="14"/>
+      <c r="FN36" s="16"/>
+      <c r="FO36" s="16"/>
+      <c r="FP36" s="16"/>
+      <c r="FQ36" s="16"/>
+      <c r="FR36" s="16"/>
+      <c r="FS36" s="14"/>
+      <c r="FT36" s="14"/>
+      <c r="FU36" s="16"/>
+      <c r="FV36" s="16"/>
+      <c r="FW36" s="16"/>
+      <c r="FX36" s="16"/>
+      <c r="FY36" s="16"/>
+      <c r="FZ36" s="149"/>
     </row>
-    <row r="37" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="123"/>
       <c r="B37" s="24"/>
       <c r="C37" s="16"/>
@@ -16787,8 +17825,38 @@
       <c r="ET37" s="13"/>
       <c r="EU37" s="13"/>
       <c r="EV37" s="17"/>
+      <c r="EW37" s="67"/>
+      <c r="EX37" s="14"/>
+      <c r="EY37" s="14"/>
+      <c r="EZ37" s="16"/>
+      <c r="FA37" s="16"/>
+      <c r="FB37" s="14"/>
+      <c r="FC37" s="16"/>
+      <c r="FD37" s="16"/>
+      <c r="FE37" s="14"/>
+      <c r="FF37" s="14"/>
+      <c r="FG37" s="16"/>
+      <c r="FH37" s="16"/>
+      <c r="FI37" s="14"/>
+      <c r="FJ37" s="16"/>
+      <c r="FK37" s="16"/>
+      <c r="FL37" s="14"/>
+      <c r="FM37" s="14"/>
+      <c r="FN37" s="16"/>
+      <c r="FO37" s="16"/>
+      <c r="FP37" s="16"/>
+      <c r="FQ37" s="16"/>
+      <c r="FR37" s="16"/>
+      <c r="FS37" s="14"/>
+      <c r="FT37" s="14"/>
+      <c r="FU37" s="16"/>
+      <c r="FV37" s="16"/>
+      <c r="FW37" s="16"/>
+      <c r="FX37" s="16"/>
+      <c r="FY37" s="16"/>
+      <c r="FZ37" s="149"/>
     </row>
-    <row r="38" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="123"/>
       <c r="B38" s="24"/>
       <c r="C38" s="16"/>
@@ -16941,8 +18009,38 @@
       <c r="ET38" s="13"/>
       <c r="EU38" s="13"/>
       <c r="EV38" s="17"/>
+      <c r="EW38" s="67"/>
+      <c r="EX38" s="14"/>
+      <c r="EY38" s="14"/>
+      <c r="EZ38" s="16"/>
+      <c r="FA38" s="16"/>
+      <c r="FB38" s="14"/>
+      <c r="FC38" s="16"/>
+      <c r="FD38" s="16"/>
+      <c r="FE38" s="14"/>
+      <c r="FF38" s="14"/>
+      <c r="FG38" s="16"/>
+      <c r="FH38" s="16"/>
+      <c r="FI38" s="14"/>
+      <c r="FJ38" s="16"/>
+      <c r="FK38" s="16"/>
+      <c r="FL38" s="14"/>
+      <c r="FM38" s="14"/>
+      <c r="FN38" s="16"/>
+      <c r="FO38" s="16"/>
+      <c r="FP38" s="16"/>
+      <c r="FQ38" s="16"/>
+      <c r="FR38" s="16"/>
+      <c r="FS38" s="14"/>
+      <c r="FT38" s="14"/>
+      <c r="FU38" s="16"/>
+      <c r="FV38" s="16"/>
+      <c r="FW38" s="16"/>
+      <c r="FX38" s="16"/>
+      <c r="FY38" s="16"/>
+      <c r="FZ38" s="149"/>
     </row>
-    <row r="39" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:182" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="123"/>
       <c r="B39" s="85"/>
       <c r="C39" s="71"/>
@@ -17095,8 +18193,38 @@
       <c r="ET39" s="73"/>
       <c r="EU39" s="73"/>
       <c r="EV39" s="98"/>
+      <c r="EW39" s="70"/>
+      <c r="EX39" s="72"/>
+      <c r="EY39" s="72"/>
+      <c r="EZ39" s="71"/>
+      <c r="FA39" s="71"/>
+      <c r="FB39" s="72"/>
+      <c r="FC39" s="71"/>
+      <c r="FD39" s="71"/>
+      <c r="FE39" s="72"/>
+      <c r="FF39" s="72"/>
+      <c r="FG39" s="71"/>
+      <c r="FH39" s="71"/>
+      <c r="FI39" s="72"/>
+      <c r="FJ39" s="71"/>
+      <c r="FK39" s="71"/>
+      <c r="FL39" s="72"/>
+      <c r="FM39" s="72"/>
+      <c r="FN39" s="71"/>
+      <c r="FO39" s="71"/>
+      <c r="FP39" s="71"/>
+      <c r="FQ39" s="71"/>
+      <c r="FR39" s="71"/>
+      <c r="FS39" s="72"/>
+      <c r="FT39" s="72"/>
+      <c r="FU39" s="71"/>
+      <c r="FV39" s="71"/>
+      <c r="FW39" s="71"/>
+      <c r="FX39" s="71"/>
+      <c r="FY39" s="71"/>
+      <c r="FZ39" s="152"/>
     </row>
-    <row r="40" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="122" t="s">
         <v>22</v>
       </c>
@@ -17204,9 +18332,7 @@
       <c r="CU40" s="77"/>
       <c r="CV40" s="46"/>
       <c r="CW40" s="76"/>
-      <c r="CX40" s="46" t="s">
-        <v>9</v>
-      </c>
+      <c r="CX40" s="46"/>
       <c r="CY40" s="76"/>
       <c r="CZ40" s="76"/>
       <c r="DA40" s="77"/>
@@ -17228,11 +18354,13 @@
       <c r="DQ40" s="84"/>
       <c r="DR40" s="82"/>
       <c r="DS40" s="76"/>
-      <c r="DT40" s="76"/>
-      <c r="DU40" s="76"/>
-      <c r="DV40" s="77"/>
-      <c r="DW40" s="77"/>
-      <c r="DX40" s="77"/>
+      <c r="DT40" s="134" t="s">
+        <v>9</v>
+      </c>
+      <c r="DU40" s="88"/>
+      <c r="DV40" s="88"/>
+      <c r="DW40" s="88"/>
+      <c r="DX40" s="88"/>
       <c r="DY40" s="76"/>
       <c r="DZ40" s="76"/>
       <c r="EA40" s="76"/>
@@ -17248,17 +18376,49 @@
       <c r="EK40" s="77"/>
       <c r="EL40" s="78"/>
       <c r="EM40" s="77"/>
-      <c r="EN40" s="76"/>
-      <c r="EO40" s="76"/>
-      <c r="EP40" s="76"/>
-      <c r="EQ40" s="77"/>
-      <c r="ER40" s="77"/>
-      <c r="ES40" s="78"/>
-      <c r="ET40" s="78"/>
+      <c r="EN40" s="88" t="s">
+        <v>2</v>
+      </c>
+      <c r="EO40" s="88"/>
+      <c r="EP40" s="88"/>
+      <c r="EQ40" s="88"/>
+      <c r="ER40" s="135"/>
+      <c r="ES40" s="136"/>
+      <c r="ET40" s="88"/>
       <c r="EU40" s="78"/>
       <c r="EV40" s="102"/>
+      <c r="EW40" s="82"/>
+      <c r="EX40" s="77"/>
+      <c r="EY40" s="77"/>
+      <c r="EZ40" s="76"/>
+      <c r="FA40" s="76"/>
+      <c r="FB40" s="77"/>
+      <c r="FC40" s="76"/>
+      <c r="FD40" s="76"/>
+      <c r="FE40" s="142"/>
+      <c r="FF40" s="77"/>
+      <c r="FG40" s="46"/>
+      <c r="FH40" s="76"/>
+      <c r="FI40" s="77"/>
+      <c r="FJ40" s="76"/>
+      <c r="FK40" s="76"/>
+      <c r="FL40" s="77"/>
+      <c r="FM40" s="77"/>
+      <c r="FN40" s="76"/>
+      <c r="FO40" s="76"/>
+      <c r="FP40" s="76"/>
+      <c r="FQ40" s="76"/>
+      <c r="FR40" s="76"/>
+      <c r="FS40" s="77"/>
+      <c r="FT40" s="77"/>
+      <c r="FU40" s="76"/>
+      <c r="FV40" s="76"/>
+      <c r="FW40" s="76"/>
+      <c r="FX40" s="76"/>
+      <c r="FY40" s="76"/>
+      <c r="FZ40" s="151"/>
     </row>
-    <row r="41" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="123"/>
       <c r="B41" s="24"/>
       <c r="C41" s="16"/>
@@ -17360,9 +18520,7 @@
       <c r="CU41" s="14"/>
       <c r="CV41" s="13"/>
       <c r="CW41" s="16"/>
-      <c r="CX41" s="16" t="s">
-        <v>64</v>
-      </c>
+      <c r="CX41" s="16"/>
       <c r="CY41" s="16"/>
       <c r="CZ41" s="16"/>
       <c r="DA41" s="14"/>
@@ -17384,11 +18542,13 @@
       <c r="DQ41" s="25"/>
       <c r="DR41" s="67"/>
       <c r="DS41" s="16"/>
-      <c r="DT41" s="16"/>
-      <c r="DU41" s="16"/>
-      <c r="DV41" s="14"/>
-      <c r="DW41" s="14"/>
-      <c r="DX41" s="14"/>
+      <c r="DT41" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="DU41" s="59"/>
+      <c r="DV41" s="59"/>
+      <c r="DW41" s="59"/>
+      <c r="DX41" s="59"/>
       <c r="DY41" s="16"/>
       <c r="DZ41" s="16"/>
       <c r="EA41" s="16"/>
@@ -17413,8 +18573,38 @@
       <c r="ET41" s="13"/>
       <c r="EU41" s="13"/>
       <c r="EV41" s="17"/>
+      <c r="EW41" s="67"/>
+      <c r="EX41" s="14"/>
+      <c r="EY41" s="14"/>
+      <c r="EZ41" s="16"/>
+      <c r="FA41" s="16"/>
+      <c r="FB41" s="14"/>
+      <c r="FC41" s="16"/>
+      <c r="FD41" s="16"/>
+      <c r="FE41" s="14"/>
+      <c r="FF41" s="14"/>
+      <c r="FG41" s="16"/>
+      <c r="FH41" s="16"/>
+      <c r="FI41" s="14"/>
+      <c r="FJ41" s="16"/>
+      <c r="FK41" s="16"/>
+      <c r="FL41" s="140"/>
+      <c r="FM41" s="14"/>
+      <c r="FN41" s="16"/>
+      <c r="FO41" s="16"/>
+      <c r="FP41" s="16"/>
+      <c r="FQ41" s="16"/>
+      <c r="FR41" s="16"/>
+      <c r="FS41" s="14"/>
+      <c r="FT41" s="14"/>
+      <c r="FU41" s="16"/>
+      <c r="FV41" s="16"/>
+      <c r="FW41" s="16"/>
+      <c r="FX41" s="16"/>
+      <c r="FY41" s="16"/>
+      <c r="FZ41" s="149"/>
     </row>
-    <row r="42" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="123"/>
       <c r="B42" s="24"/>
       <c r="C42" s="16"/>
@@ -17489,7 +18679,7 @@
       <c r="BT42" s="13"/>
       <c r="BU42" s="16"/>
       <c r="BV42" s="56" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="BW42" s="16"/>
       <c r="BX42" s="16"/>
@@ -17520,9 +18710,7 @@
       <c r="CU42" s="14"/>
       <c r="CV42" s="13"/>
       <c r="CW42" s="16"/>
-      <c r="CX42" s="16" t="s">
-        <v>54</v>
-      </c>
+      <c r="CX42" s="16"/>
       <c r="CY42" s="16"/>
       <c r="CZ42" s="16"/>
       <c r="DA42" s="14"/>
@@ -17549,7 +18737,9 @@
       <c r="DV42" s="14"/>
       <c r="DW42" s="14"/>
       <c r="DX42" s="14"/>
-      <c r="DY42" s="16"/>
+      <c r="DY42" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="DZ42" s="16"/>
       <c r="EA42" s="16"/>
       <c r="EB42" s="16"/>
@@ -17561,9 +18751,11 @@
       <c r="EH42" s="16"/>
       <c r="EI42" s="16"/>
       <c r="EJ42" s="14"/>
-      <c r="EK42" s="14"/>
-      <c r="EL42" s="13"/>
-      <c r="EM42" s="14"/>
+      <c r="EK42" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="EL42" s="59"/>
+      <c r="EM42" s="59"/>
       <c r="EN42" s="16"/>
       <c r="EO42" s="16"/>
       <c r="EP42" s="16"/>
@@ -17573,8 +18765,38 @@
       <c r="ET42" s="13"/>
       <c r="EU42" s="13"/>
       <c r="EV42" s="17"/>
+      <c r="EW42" s="67"/>
+      <c r="EX42" s="14"/>
+      <c r="EY42" s="14"/>
+      <c r="EZ42" s="16"/>
+      <c r="FA42" s="16"/>
+      <c r="FB42" s="14"/>
+      <c r="FC42" s="16"/>
+      <c r="FD42" s="16"/>
+      <c r="FE42" s="14"/>
+      <c r="FF42" s="14"/>
+      <c r="FG42" s="16"/>
+      <c r="FH42" s="16"/>
+      <c r="FI42" s="14"/>
+      <c r="FJ42" s="16"/>
+      <c r="FK42" s="16"/>
+      <c r="FL42" s="14"/>
+      <c r="FM42" s="14"/>
+      <c r="FN42" s="16"/>
+      <c r="FO42" s="16"/>
+      <c r="FP42" s="16"/>
+      <c r="FQ42" s="16"/>
+      <c r="FR42" s="16"/>
+      <c r="FS42" s="14"/>
+      <c r="FT42" s="14"/>
+      <c r="FU42" s="16"/>
+      <c r="FV42" s="16"/>
+      <c r="FW42" s="16"/>
+      <c r="FX42" s="16"/>
+      <c r="FY42" s="16"/>
+      <c r="FZ42" s="149"/>
     </row>
-    <row r="43" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="123"/>
       <c r="B43" s="24"/>
       <c r="C43" s="16"/>
@@ -17681,9 +18903,7 @@
       <c r="CZ43" s="16"/>
       <c r="DA43" s="14"/>
       <c r="DB43" s="14"/>
-      <c r="DC43" s="23" t="s">
-        <v>53</v>
-      </c>
+      <c r="DC43" s="23"/>
       <c r="DD43" s="16"/>
       <c r="DE43" s="16"/>
       <c r="DF43" s="16"/>
@@ -17692,9 +18912,7 @@
       <c r="DI43" s="14"/>
       <c r="DJ43" s="23"/>
       <c r="DK43" s="16"/>
-      <c r="DL43" s="16" t="s">
-        <v>66</v>
-      </c>
+      <c r="DL43" s="16"/>
       <c r="DM43" s="16"/>
       <c r="DN43" s="16"/>
       <c r="DO43" s="14"/>
@@ -17707,7 +18925,9 @@
       <c r="DV43" s="14"/>
       <c r="DW43" s="14"/>
       <c r="DX43" s="14"/>
-      <c r="DY43" s="16"/>
+      <c r="DY43" s="133" t="s">
+        <v>53</v>
+      </c>
       <c r="DZ43" s="16"/>
       <c r="EA43" s="16"/>
       <c r="EB43" s="16"/>
@@ -17731,8 +18951,38 @@
       <c r="ET43" s="13"/>
       <c r="EU43" s="13"/>
       <c r="EV43" s="17"/>
+      <c r="EW43" s="67"/>
+      <c r="EX43" s="14"/>
+      <c r="EY43" s="14"/>
+      <c r="EZ43" s="16"/>
+      <c r="FA43" s="16"/>
+      <c r="FB43" s="14"/>
+      <c r="FC43" s="16"/>
+      <c r="FD43" s="16"/>
+      <c r="FE43" s="14"/>
+      <c r="FF43" s="14"/>
+      <c r="FG43" s="16"/>
+      <c r="FH43" s="16"/>
+      <c r="FI43" s="14"/>
+      <c r="FJ43" s="16"/>
+      <c r="FK43" s="16"/>
+      <c r="FL43" s="140"/>
+      <c r="FM43" s="14"/>
+      <c r="FN43" s="16"/>
+      <c r="FO43" s="16"/>
+      <c r="FP43" s="16"/>
+      <c r="FQ43" s="16"/>
+      <c r="FR43" s="16"/>
+      <c r="FS43" s="140"/>
+      <c r="FT43" s="14"/>
+      <c r="FU43" s="16"/>
+      <c r="FV43" s="16"/>
+      <c r="FW43" s="16"/>
+      <c r="FX43" s="16"/>
+      <c r="FY43" s="16"/>
+      <c r="FZ43" s="149"/>
     </row>
-    <row r="44" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:182" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="124"/>
       <c r="B44" s="85"/>
       <c r="C44" s="71"/>
@@ -17885,8 +19135,38 @@
       <c r="ET44" s="73"/>
       <c r="EU44" s="73"/>
       <c r="EV44" s="98"/>
+      <c r="EW44" s="70"/>
+      <c r="EX44" s="72"/>
+      <c r="EY44" s="72"/>
+      <c r="EZ44" s="71"/>
+      <c r="FA44" s="71"/>
+      <c r="FB44" s="72"/>
+      <c r="FC44" s="71"/>
+      <c r="FD44" s="71"/>
+      <c r="FE44" s="14"/>
+      <c r="FF44" s="72"/>
+      <c r="FG44" s="71"/>
+      <c r="FH44" s="71"/>
+      <c r="FI44" s="72"/>
+      <c r="FJ44" s="71"/>
+      <c r="FK44" s="71"/>
+      <c r="FL44" s="72"/>
+      <c r="FM44" s="72"/>
+      <c r="FN44" s="71"/>
+      <c r="FO44" s="71"/>
+      <c r="FP44" s="71"/>
+      <c r="FQ44" s="71"/>
+      <c r="FR44" s="71"/>
+      <c r="FS44" s="72"/>
+      <c r="FT44" s="72"/>
+      <c r="FU44" s="71"/>
+      <c r="FV44" s="71"/>
+      <c r="FW44" s="71"/>
+      <c r="FX44" s="71"/>
+      <c r="FY44" s="71"/>
+      <c r="FZ44" s="152"/>
     </row>
-    <row r="45" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="123" t="s">
         <v>24</v>
       </c>
@@ -18047,8 +19327,38 @@
       <c r="ET45" s="78"/>
       <c r="EU45" s="78"/>
       <c r="EV45" s="102"/>
+      <c r="EW45" s="82"/>
+      <c r="EX45" s="141"/>
+      <c r="EY45" s="77"/>
+      <c r="EZ45" s="76"/>
+      <c r="FA45" s="76"/>
+      <c r="FB45" s="77"/>
+      <c r="FC45" s="76"/>
+      <c r="FD45" s="76"/>
+      <c r="FE45" s="77"/>
+      <c r="FF45" s="77"/>
+      <c r="FG45" s="76"/>
+      <c r="FH45" s="76"/>
+      <c r="FI45" s="77"/>
+      <c r="FJ45" s="76"/>
+      <c r="FK45" s="76"/>
+      <c r="FL45" s="143"/>
+      <c r="FM45" s="77"/>
+      <c r="FN45" s="76"/>
+      <c r="FO45" s="76"/>
+      <c r="FP45" s="76"/>
+      <c r="FQ45" s="76"/>
+      <c r="FR45" s="76"/>
+      <c r="FS45" s="77"/>
+      <c r="FT45" s="77"/>
+      <c r="FU45" s="76"/>
+      <c r="FV45" s="76"/>
+      <c r="FW45" s="76"/>
+      <c r="FX45" s="76"/>
+      <c r="FY45" s="76"/>
+      <c r="FZ45" s="151"/>
     </row>
-    <row r="46" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="123"/>
       <c r="B46" s="24"/>
       <c r="C46" s="16"/>
@@ -18201,8 +19511,38 @@
       <c r="ET46" s="13"/>
       <c r="EU46" s="13"/>
       <c r="EV46" s="17"/>
+      <c r="EW46" s="67"/>
+      <c r="EX46" s="14"/>
+      <c r="EY46" s="14"/>
+      <c r="EZ46" s="16"/>
+      <c r="FA46" s="16"/>
+      <c r="FB46" s="14"/>
+      <c r="FC46" s="16"/>
+      <c r="FD46" s="16"/>
+      <c r="FE46" s="14"/>
+      <c r="FF46" s="14"/>
+      <c r="FG46" s="16"/>
+      <c r="FH46" s="16"/>
+      <c r="FI46" s="14"/>
+      <c r="FJ46" s="16"/>
+      <c r="FK46" s="16"/>
+      <c r="FL46" s="14"/>
+      <c r="FM46" s="14"/>
+      <c r="FN46" s="16"/>
+      <c r="FO46" s="16"/>
+      <c r="FP46" s="16"/>
+      <c r="FQ46" s="16"/>
+      <c r="FR46" s="16"/>
+      <c r="FS46" s="14"/>
+      <c r="FT46" s="14"/>
+      <c r="FU46" s="16"/>
+      <c r="FV46" s="16"/>
+      <c r="FW46" s="16"/>
+      <c r="FX46" s="16"/>
+      <c r="FY46" s="16"/>
+      <c r="FZ46" s="149"/>
     </row>
-    <row r="47" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="123"/>
       <c r="B47" s="24"/>
       <c r="C47" s="16"/>
@@ -18337,7 +19677,7 @@
       <c r="EB47" s="16"/>
       <c r="EC47" s="14"/>
       <c r="ED47" s="14"/>
-      <c r="EE47" s="14"/>
+      <c r="EE47" s="13"/>
       <c r="EF47" s="16"/>
       <c r="EG47" s="16"/>
       <c r="EH47" s="16"/>
@@ -18355,8 +19695,38 @@
       <c r="ET47" s="13"/>
       <c r="EU47" s="13"/>
       <c r="EV47" s="17"/>
+      <c r="EW47" s="67"/>
+      <c r="EX47" s="14"/>
+      <c r="EY47" s="14"/>
+      <c r="EZ47" s="16"/>
+      <c r="FA47" s="16"/>
+      <c r="FB47" s="14"/>
+      <c r="FC47" s="16"/>
+      <c r="FD47" s="16"/>
+      <c r="FE47" s="14"/>
+      <c r="FF47" s="14"/>
+      <c r="FG47" s="16"/>
+      <c r="FH47" s="16"/>
+      <c r="FI47" s="14"/>
+      <c r="FJ47" s="16"/>
+      <c r="FK47" s="16"/>
+      <c r="FL47" s="14"/>
+      <c r="FM47" s="14"/>
+      <c r="FN47" s="16"/>
+      <c r="FO47" s="16"/>
+      <c r="FP47" s="16"/>
+      <c r="FQ47" s="16"/>
+      <c r="FR47" s="16"/>
+      <c r="FS47" s="14"/>
+      <c r="FT47" s="14"/>
+      <c r="FU47" s="16"/>
+      <c r="FV47" s="16"/>
+      <c r="FW47" s="16"/>
+      <c r="FX47" s="16"/>
+      <c r="FY47" s="16"/>
+      <c r="FZ47" s="14"/>
     </row>
-    <row r="48" spans="1:152" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:182" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="123"/>
       <c r="B48" s="24"/>
       <c r="C48" s="16"/>
@@ -18509,8 +19879,38 @@
       <c r="ET48" s="13"/>
       <c r="EU48" s="13"/>
       <c r="EV48" s="17"/>
+      <c r="EW48" s="67"/>
+      <c r="EX48" s="14"/>
+      <c r="EY48" s="14"/>
+      <c r="EZ48" s="16"/>
+      <c r="FA48" s="16"/>
+      <c r="FB48" s="14"/>
+      <c r="FC48" s="16"/>
+      <c r="FD48" s="16"/>
+      <c r="FE48" s="14"/>
+      <c r="FF48" s="14"/>
+      <c r="FG48" s="16"/>
+      <c r="FH48" s="16"/>
+      <c r="FI48" s="14"/>
+      <c r="FJ48" s="16"/>
+      <c r="FK48" s="16"/>
+      <c r="FL48" s="14"/>
+      <c r="FM48" s="14"/>
+      <c r="FN48" s="16"/>
+      <c r="FO48" s="16"/>
+      <c r="FP48" s="16"/>
+      <c r="FQ48" s="16"/>
+      <c r="FR48" s="16"/>
+      <c r="FS48" s="14"/>
+      <c r="FT48" s="14"/>
+      <c r="FU48" s="16"/>
+      <c r="FV48" s="23"/>
+      <c r="FW48" s="16"/>
+      <c r="FX48" s="16"/>
+      <c r="FY48" s="16"/>
+      <c r="FZ48" s="140"/>
     </row>
-    <row r="49" spans="1:152" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:182" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="124"/>
       <c r="B49" s="85"/>
       <c r="C49" s="71"/>
@@ -18663,26 +20063,63 @@
       <c r="ET49" s="73"/>
       <c r="EU49" s="73"/>
       <c r="EV49" s="98"/>
+      <c r="EW49" s="70"/>
+      <c r="EX49" s="72"/>
+      <c r="EY49" s="72"/>
+      <c r="EZ49" s="71"/>
+      <c r="FA49" s="71"/>
+      <c r="FB49" s="72"/>
+      <c r="FC49" s="71"/>
+      <c r="FD49" s="71"/>
+      <c r="FE49" s="72"/>
+      <c r="FF49" s="72"/>
+      <c r="FG49" s="71"/>
+      <c r="FH49" s="71"/>
+      <c r="FI49" s="72"/>
+      <c r="FJ49" s="71"/>
+      <c r="FK49" s="71"/>
+      <c r="FL49" s="72"/>
+      <c r="FM49" s="72"/>
+      <c r="FN49" s="71"/>
+      <c r="FO49" s="71"/>
+      <c r="FP49" s="71"/>
+      <c r="FQ49" s="71"/>
+      <c r="FR49" s="71"/>
+      <c r="FS49" s="72"/>
+      <c r="FT49" s="72"/>
+      <c r="FU49" s="71"/>
+      <c r="FV49" s="71"/>
+      <c r="FW49" s="71"/>
+      <c r="FX49" s="71"/>
+      <c r="FY49" s="71"/>
+      <c r="FZ49" s="152"/>
     </row>
-    <row r="50" spans="1:152" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:152" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:152" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:152" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:152" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:152" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:152" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:152" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:152" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:152" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:152" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:152" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:152" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:152" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:152" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:182" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:182" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:182" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:182" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:182" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:182" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:182" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:182" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:182" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:182" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:182" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:182" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:182" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:182" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:182" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="65" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="66" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="EW6:FZ6"/>
+    <mergeCell ref="B6:AF6"/>
+    <mergeCell ref="AG6:BH6"/>
+    <mergeCell ref="BI6:CM6"/>
+    <mergeCell ref="CN6:DQ6"/>
+    <mergeCell ref="DR6:EV6"/>
     <mergeCell ref="A45:A49"/>
     <mergeCell ref="A15:A19"/>
     <mergeCell ref="A20:A24"/>
@@ -18690,16 +20127,11 @@
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="A35:A39"/>
     <mergeCell ref="A40:A44"/>
-    <mergeCell ref="B6:AF6"/>
-    <mergeCell ref="AG6:BH6"/>
-    <mergeCell ref="BI6:CM6"/>
-    <mergeCell ref="CN6:DQ6"/>
-    <mergeCell ref="DR6:EV6"/>
-    <mergeCell ref="A8:A14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Pipette] DC Jack 추가, file name 통일
</commit_message>
<xml_diff>
--- a/0_DOC/Femto Project schedule V1.0.xlsx
+++ b/0_DOC/Femto Project schedule V1.0.xlsx
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="111">
   <si>
     <t>◇PCB설계</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -523,10 +523,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>S/V 연결부품 검토</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>니들 type 검토</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -571,11 +567,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>▶WIFI 기능 추가 검토</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S/V 및 Fitting 검토</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>▶계룡 사무실 Open</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>▶WIFI 기능 추가 검토</t>
+    <t>▶기구 부품 입고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S/V 및 부자재</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fitting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>니들</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5369,6 +5385,161 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>97</xdr:col>
+      <xdr:colOff>77444</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>89577</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>105</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>89577</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="54" name="직선 화살표 연결선 53"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20472150" y="885195"/>
+          <a:ext cx="1726703" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>96</xdr:col>
+      <xdr:colOff>128991</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>96301</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>105</xdr:col>
+      <xdr:colOff>179294</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>96301</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="58" name="직선 화살표 연결선 57"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20321991" y="1071213"/>
+          <a:ext cx="1865656" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>106</xdr:col>
+      <xdr:colOff>116919</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>39970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>106</xdr:col>
+      <xdr:colOff>129619</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>118408</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="63" name="꺾인 연결선 62"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="20971815" y="2190751"/>
+          <a:ext cx="2723026" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -12971,7 +13142,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CE1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DG21" sqref="DG21"/>
+      <selection pane="topRight" activeCell="DT10" sqref="DT10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -14601,7 +14772,7 @@
       <c r="CL8" s="35"/>
       <c r="CM8" s="133"/>
       <c r="CN8" s="61" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="CO8" s="49"/>
       <c r="CP8" s="35"/>
@@ -14617,7 +14788,9 @@
       <c r="CZ8" s="35"/>
       <c r="DA8" s="38"/>
       <c r="DB8" s="38"/>
-      <c r="DC8" s="49"/>
+      <c r="DC8" s="49" t="s">
+        <v>107</v>
+      </c>
       <c r="DD8" s="35"/>
       <c r="DE8" s="36"/>
       <c r="DF8" s="35"/>
@@ -14746,7 +14919,7 @@
       <c r="HW8" s="38"/>
       <c r="HX8" s="38"/>
       <c r="HY8" s="49" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="HZ8" s="35"/>
       <c r="IA8" s="36"/>
@@ -14984,7 +15157,7 @@
       <c r="CM9" s="31"/>
       <c r="CN9" s="29"/>
       <c r="CO9" s="28" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="CP9" s="30"/>
       <c r="CQ9" s="30"/>
@@ -15000,7 +15173,9 @@
       <c r="DA9" s="31"/>
       <c r="DB9" s="31"/>
       <c r="DC9" s="28"/>
-      <c r="DD9" s="30"/>
+      <c r="DD9" s="30" t="s">
+        <v>108</v>
+      </c>
       <c r="DE9" s="30"/>
       <c r="DF9" s="30"/>
       <c r="DG9" s="30"/>
@@ -15362,7 +15537,7 @@
       <c r="CM10" s="31"/>
       <c r="CN10" s="29"/>
       <c r="CO10" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CP10" s="30"/>
       <c r="CQ10" s="30"/>
@@ -15378,7 +15553,9 @@
       <c r="DA10" s="31"/>
       <c r="DB10" s="31"/>
       <c r="DC10" s="28"/>
-      <c r="DD10" s="30"/>
+      <c r="DD10" s="30" t="s">
+        <v>109</v>
+      </c>
       <c r="DE10" s="30"/>
       <c r="DF10" s="30"/>
       <c r="DG10" s="30"/>
@@ -15736,7 +15913,7 @@
       <c r="CM11" s="31"/>
       <c r="CN11" s="29"/>
       <c r="CO11" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="CP11" s="30"/>
       <c r="CQ11" s="30"/>
@@ -15752,7 +15929,9 @@
       <c r="DA11" s="31"/>
       <c r="DB11" s="31"/>
       <c r="DC11" s="28"/>
-      <c r="DD11" s="30"/>
+      <c r="DD11" s="30" t="s">
+        <v>110</v>
+      </c>
       <c r="DE11" s="30"/>
       <c r="DF11" s="30"/>
       <c r="DG11" s="30"/>
@@ -16110,7 +16289,7 @@
       <c r="CM12" s="31"/>
       <c r="CN12" s="29"/>
       <c r="CO12" s="28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="CP12" s="30"/>
       <c r="CQ12" s="30"/>
@@ -17228,7 +17407,7 @@
       <c r="CM15" s="44"/>
       <c r="CN15" s="42"/>
       <c r="CO15" s="45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="CP15" s="43"/>
       <c r="CQ15" s="43"/>
@@ -23207,7 +23386,7 @@
       <c r="CT31" s="14"/>
       <c r="CU31" s="14"/>
       <c r="CV31" s="154" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="CW31" s="16"/>
       <c r="CX31" s="16"/>
@@ -23349,7 +23528,7 @@
       <c r="ID31" s="14"/>
       <c r="IE31" s="14"/>
       <c r="IF31" s="154" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="IG31" s="16"/>
       <c r="IH31" s="16"/>
@@ -23414,7 +23593,7 @@
       <c r="KO31" s="14"/>
       <c r="KP31" s="14"/>
       <c r="KQ31" s="154" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="KR31" s="16"/>
       <c r="KS31" s="25"/>
@@ -23582,7 +23761,7 @@
       <c r="CU32" s="14"/>
       <c r="CV32" s="13"/>
       <c r="CW32" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="CX32" s="16"/>
       <c r="CY32" s="16"/>
@@ -23724,7 +23903,7 @@
       <c r="IE32" s="14"/>
       <c r="IF32" s="154"/>
       <c r="IG32" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="IH32" s="16"/>
       <c r="II32" s="16"/>
@@ -23789,7 +23968,7 @@
       <c r="KP32" s="14"/>
       <c r="KQ32" s="16"/>
       <c r="KR32" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="KS32" s="25"/>
       <c r="KT32" s="67"/>
@@ -24159,7 +24338,7 @@
       <c r="KP33" s="14"/>
       <c r="KQ33" s="16"/>
       <c r="KR33" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="KS33" s="25"/>
       <c r="KT33" s="67"/>
@@ -32085,6 +32264,11 @@
     <row r="71" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="GA6:HE6"/>
+    <mergeCell ref="HF6:IJ6"/>
+    <mergeCell ref="IK6:JN6"/>
+    <mergeCell ref="JO6:KS6"/>
+    <mergeCell ref="KT6:LW6"/>
     <mergeCell ref="LX6:NB6"/>
     <mergeCell ref="A50:A54"/>
     <mergeCell ref="A15:A19"/>
@@ -32101,11 +32285,6 @@
     <mergeCell ref="BI6:CM6"/>
     <mergeCell ref="CN6:DQ6"/>
     <mergeCell ref="DR6:EV6"/>
-    <mergeCell ref="GA6:HE6"/>
-    <mergeCell ref="HF6:IJ6"/>
-    <mergeCell ref="IK6:JN6"/>
-    <mergeCell ref="JO6:KS6"/>
-    <mergeCell ref="KT6:LW6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[DOC] LF GEN 일정 및 비용 update
</commit_message>
<xml_diff>
--- a/0_DOC/Femto Project schedule V1.0.xlsx
+++ b/0_DOC/Femto Project schedule V1.0.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="1"/>
@@ -14,7 +14,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'20180207'!$A$1:$EH$49</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'20180328'!$A$1:$ND$54</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -24,7 +24,7 @@
     <author>만든 이</author>
   </authors>
   <commentList>
-    <comment ref="EM7" authorId="0" shapeId="0">
+    <comment ref="EM7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -39,7 +39,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FB7" authorId="0" shapeId="0">
+    <comment ref="FB7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FI7" authorId="0" shapeId="0">
+    <comment ref="FI7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -69,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="HT7" authorId="0" shapeId="0">
+    <comment ref="HT7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -84,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="JH7" authorId="0" shapeId="0">
+    <comment ref="JH7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -99,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="JQ7" authorId="0" shapeId="0">
+    <comment ref="JQ7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -114,7 +114,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="JW7" authorId="0" shapeId="0">
+    <comment ref="JW7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -129,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="MV7" authorId="0" shapeId="0">
+    <comment ref="MV7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -420,10 +420,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>◇회로설계</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>◇장비 기능 검토</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -596,6 +592,10 @@
   </si>
   <si>
     <t>◇Batt CON sample 발주</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>◇장비검토</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1243,7 +1243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1475,6 +1475,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -3510,15 +3511,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>100</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>84535</xdr:rowOff>
+      <xdr:colOff>117661</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>73330</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>110</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>84535</xdr:rowOff>
+      <xdr:col>111</xdr:col>
+      <xdr:colOff>11205</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>73330</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3527,7 +3528,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="21095074" y="6214153"/>
+          <a:off x="21117485" y="6371036"/>
           <a:ext cx="2112308" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -4196,16 +4197,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>119</xdr:col>
-      <xdr:colOff>115544</xdr:colOff>
+      <xdr:col>104</xdr:col>
+      <xdr:colOff>126749</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>94060</xdr:rowOff>
+      <xdr:rowOff>60442</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>123</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
+      <xdr:col>108</xdr:col>
+      <xdr:colOff>182655</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>94060</xdr:rowOff>
+      <xdr:rowOff>60442</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4214,8 +4215,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="22123897" y="5887501"/>
-          <a:ext cx="862729" cy="0"/>
+          <a:off x="21933396" y="5853883"/>
+          <a:ext cx="862730" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4247,16 +4248,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>120</xdr:col>
-      <xdr:colOff>10769</xdr:colOff>
+      <xdr:col>105</xdr:col>
+      <xdr:colOff>21974</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>103585</xdr:rowOff>
+      <xdr:rowOff>69967</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>126</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
+      <xdr:col>111</xdr:col>
+      <xdr:colOff>182655</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>103585</xdr:rowOff>
+      <xdr:rowOff>69967</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4265,7 +4266,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="22220828" y="5728938"/>
+          <a:off x="22030327" y="5695320"/>
           <a:ext cx="1370916" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -5590,7 +5591,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5625,7 +5626,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -13144,9 +13145,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:NB71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CE1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DF13" sqref="DF13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AX1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DJ43" sqref="DJ43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -14776,7 +14777,7 @@
       <c r="CL8" s="35"/>
       <c r="CM8" s="133"/>
       <c r="CN8" s="61" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="CO8" s="49"/>
       <c r="CP8" s="35"/>
@@ -14793,7 +14794,7 @@
       <c r="DA8" s="38"/>
       <c r="DB8" s="38"/>
       <c r="DC8" s="49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="DD8" s="35"/>
       <c r="DE8" s="36"/>
@@ -14869,7 +14870,7 @@
       <c r="FW8" s="36"/>
       <c r="FX8" s="35"/>
       <c r="FY8" s="35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="FZ8" s="133"/>
       <c r="GA8" s="34"/>
@@ -14923,7 +14924,7 @@
       <c r="HW8" s="38"/>
       <c r="HX8" s="38"/>
       <c r="HY8" s="49" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="HZ8" s="35"/>
       <c r="IA8" s="36"/>
@@ -15161,7 +15162,7 @@
       <c r="CM9" s="31"/>
       <c r="CN9" s="29"/>
       <c r="CO9" s="28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="CP9" s="30"/>
       <c r="CQ9" s="30"/>
@@ -15178,7 +15179,7 @@
       <c r="DB9" s="31"/>
       <c r="DC9" s="28"/>
       <c r="DD9" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="DE9" s="30"/>
       <c r="DF9" s="30"/>
@@ -15541,7 +15542,7 @@
       <c r="CM10" s="31"/>
       <c r="CN10" s="29"/>
       <c r="CO10" s="28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="CP10" s="30"/>
       <c r="CQ10" s="30"/>
@@ -15558,7 +15559,7 @@
       <c r="DB10" s="31"/>
       <c r="DC10" s="28"/>
       <c r="DD10" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="DE10" s="30"/>
       <c r="DF10" s="30"/>
@@ -15917,7 +15918,7 @@
       <c r="CM11" s="31"/>
       <c r="CN11" s="29"/>
       <c r="CO11" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CP11" s="30"/>
       <c r="CQ11" s="30"/>
@@ -15934,7 +15935,7 @@
       <c r="DB11" s="31"/>
       <c r="DC11" s="28"/>
       <c r="DD11" s="30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="DE11" s="30"/>
       <c r="DF11" s="30"/>
@@ -16293,7 +16294,7 @@
       <c r="CM12" s="31"/>
       <c r="CN12" s="29"/>
       <c r="CO12" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="CP12" s="30"/>
       <c r="CQ12" s="30"/>
@@ -17036,7 +17037,7 @@
       <c r="CP14" s="51"/>
       <c r="CQ14" s="51"/>
       <c r="CR14" s="51"/>
-      <c r="CS14" s="51" t="s">
+      <c r="CS14" s="175" t="s">
         <v>64</v>
       </c>
       <c r="CT14" s="52"/>
@@ -17395,7 +17396,7 @@
       <c r="BY15" s="44"/>
       <c r="BZ15" s="44"/>
       <c r="CA15" s="55" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="CB15" s="43"/>
       <c r="CC15" s="43"/>
@@ -17411,7 +17412,7 @@
       <c r="CM15" s="44"/>
       <c r="CN15" s="42"/>
       <c r="CO15" s="54" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="CP15" s="43"/>
       <c r="CQ15" s="43"/>
@@ -17794,7 +17795,7 @@
       <c r="CN16" s="24"/>
       <c r="CO16" s="23"/>
       <c r="CP16" s="56" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="CQ16" s="16"/>
       <c r="CR16" s="16"/>
@@ -17841,7 +17842,7 @@
       <c r="EE16" s="13"/>
       <c r="EF16" s="16"/>
       <c r="EG16" s="59" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="EH16" s="16"/>
       <c r="EI16" s="16"/>
@@ -18148,7 +18149,7 @@
       <c r="BT17" s="16"/>
       <c r="BU17" s="16"/>
       <c r="BV17" s="56" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="BW17" s="16"/>
       <c r="BX17" s="16"/>
@@ -18223,7 +18224,7 @@
       <c r="EM17" s="14"/>
       <c r="EN17" s="16"/>
       <c r="EO17" s="59" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="EP17" s="16"/>
       <c r="EQ17" s="14"/>
@@ -18569,7 +18570,7 @@
       <c r="DO18" s="14"/>
       <c r="DP18" s="14"/>
       <c r="DQ18" s="122" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="DR18" s="67"/>
       <c r="DS18" s="16"/>
@@ -18580,7 +18581,7 @@
       <c r="DX18" s="14"/>
       <c r="DY18" s="16"/>
       <c r="DZ18" s="59" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="EA18" s="59"/>
       <c r="EB18" s="16"/>
@@ -18597,7 +18598,7 @@
       <c r="EM18" s="14"/>
       <c r="EN18" s="16"/>
       <c r="EO18" s="59" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="EP18" s="16"/>
       <c r="EQ18" s="14"/>
@@ -18611,7 +18612,7 @@
       <c r="EY18" s="14"/>
       <c r="EZ18" s="16"/>
       <c r="FA18" s="59" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="FB18" s="59"/>
       <c r="FC18" s="16"/>
@@ -20443,7 +20444,7 @@
       <c r="DO23" s="14"/>
       <c r="DP23" s="14"/>
       <c r="DQ23" s="122" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="DR23" s="13"/>
       <c r="DS23" s="13"/>
@@ -21164,7 +21165,7 @@
       <c r="CT25" s="77"/>
       <c r="CU25" s="77"/>
       <c r="CV25" s="88" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="CW25" s="88"/>
       <c r="CX25" s="88"/>
@@ -21203,7 +21204,7 @@
       <c r="EE25" s="78"/>
       <c r="EF25" s="76"/>
       <c r="EG25" s="88" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="EH25" s="88"/>
       <c r="EI25" s="88"/>
@@ -21242,7 +21243,7 @@
       <c r="FP25" s="76"/>
       <c r="FQ25" s="76"/>
       <c r="FR25" s="60" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="FS25" s="77"/>
       <c r="FT25" s="77"/>
@@ -21546,7 +21547,7 @@
       <c r="DB26" s="14"/>
       <c r="DC26" s="13"/>
       <c r="DD26" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="DE26" s="16"/>
       <c r="DF26" s="16"/>
@@ -21554,7 +21555,7 @@
       <c r="DH26" s="14"/>
       <c r="DI26" s="14"/>
       <c r="DJ26" s="59" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="DK26" s="59"/>
       <c r="DL26" s="59"/>
@@ -21918,7 +21919,7 @@
       <c r="DB27" s="14"/>
       <c r="DC27" s="13"/>
       <c r="DD27" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="DE27" s="16"/>
       <c r="DF27" s="16"/>
@@ -21933,7 +21934,7 @@
       <c r="DO27" s="14"/>
       <c r="DP27" s="14"/>
       <c r="DQ27" s="161" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="DR27" s="67"/>
       <c r="DS27" s="16"/>
@@ -21959,7 +21960,7 @@
       <c r="EM27" s="14"/>
       <c r="EN27" s="16"/>
       <c r="EO27" s="59" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="EP27" s="16"/>
       <c r="EQ27" s="14"/>
@@ -22292,7 +22293,7 @@
       <c r="DB28" s="14"/>
       <c r="DC28" s="13"/>
       <c r="DD28" s="30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="DE28" s="16"/>
       <c r="DF28" s="16"/>
@@ -22307,7 +22308,7 @@
       <c r="DO28" s="14"/>
       <c r="DP28" s="14"/>
       <c r="DQ28" s="161" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="DR28" s="67"/>
       <c r="DS28" s="16"/>
@@ -22688,7 +22689,7 @@
       <c r="DZ29" s="71"/>
       <c r="EA29" s="71"/>
       <c r="EB29" s="157" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="EC29" s="157"/>
       <c r="ED29" s="157"/>
@@ -23026,7 +23027,7 @@
       <c r="CR30" s="76"/>
       <c r="CS30" s="76"/>
       <c r="CT30" s="152" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="CU30" s="77"/>
       <c r="CV30" s="78"/>
@@ -23398,7 +23399,7 @@
       <c r="CT31" s="14"/>
       <c r="CU31" s="14"/>
       <c r="CV31" s="154" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="CW31" s="16"/>
       <c r="CX31" s="16"/>
@@ -23540,7 +23541,7 @@
       <c r="ID31" s="14"/>
       <c r="IE31" s="14"/>
       <c r="IF31" s="154" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="IG31" s="16"/>
       <c r="IH31" s="16"/>
@@ -23605,7 +23606,7 @@
       <c r="KO31" s="14"/>
       <c r="KP31" s="14"/>
       <c r="KQ31" s="154" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="KR31" s="16"/>
       <c r="KS31" s="25"/>
@@ -23773,7 +23774,7 @@
       <c r="CU32" s="14"/>
       <c r="CV32" s="13"/>
       <c r="CW32" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="CX32" s="16"/>
       <c r="CY32" s="16"/>
@@ -23915,7 +23916,7 @@
       <c r="IE32" s="14"/>
       <c r="IF32" s="154"/>
       <c r="IG32" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="IH32" s="16"/>
       <c r="II32" s="16"/>
@@ -23980,7 +23981,7 @@
       <c r="KP32" s="14"/>
       <c r="KQ32" s="16"/>
       <c r="KR32" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="KS32" s="25"/>
       <c r="KT32" s="67"/>
@@ -24350,7 +24351,7 @@
       <c r="KP33" s="14"/>
       <c r="KQ33" s="16"/>
       <c r="KR33" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="KS33" s="25"/>
       <c r="KT33" s="67"/>
@@ -24892,8 +24893,10 @@
       <c r="CR35" s="43"/>
       <c r="CS35" s="43"/>
       <c r="CT35" s="44"/>
-      <c r="CU35" s="44"/>
-      <c r="CV35" s="43"/>
+      <c r="CU35" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="CV35" s="54"/>
       <c r="CW35" s="43"/>
       <c r="CX35" s="43"/>
       <c r="CY35" s="43"/>
@@ -24907,10 +24910,8 @@
       <c r="DG35" s="43"/>
       <c r="DH35" s="44"/>
       <c r="DI35" s="44"/>
-      <c r="DJ35" s="60" t="s">
-        <v>67</v>
-      </c>
-      <c r="DK35" s="60"/>
+      <c r="DJ35" s="78"/>
+      <c r="DK35" s="76"/>
       <c r="DL35" s="43"/>
       <c r="DM35" s="43"/>
       <c r="DN35" s="43"/>
@@ -25266,8 +25267,10 @@
       <c r="CR36" s="16"/>
       <c r="CS36" s="16"/>
       <c r="CT36" s="14"/>
-      <c r="CU36" s="14"/>
-      <c r="CV36" s="16"/>
+      <c r="CU36" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="CV36" s="56"/>
       <c r="CW36" s="16"/>
       <c r="CX36" s="16"/>
       <c r="CY36" s="16"/>
@@ -25281,10 +25284,8 @@
       <c r="DG36" s="16"/>
       <c r="DH36" s="14"/>
       <c r="DI36" s="14"/>
-      <c r="DJ36" s="59" t="s">
-        <v>60</v>
-      </c>
-      <c r="DK36" s="59"/>
+      <c r="DJ36" s="13"/>
+      <c r="DK36" s="16"/>
       <c r="DL36" s="16"/>
       <c r="DM36" s="16"/>
       <c r="DN36" s="16"/>
@@ -25642,7 +25643,9 @@
       <c r="CT37" s="14"/>
       <c r="CU37" s="14"/>
       <c r="CV37" s="16"/>
-      <c r="CW37" s="16"/>
+      <c r="CW37" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="CX37" s="16"/>
       <c r="CY37" s="16"/>
       <c r="CZ37" s="16"/>
@@ -25657,9 +25660,7 @@
       <c r="DI37" s="14"/>
       <c r="DJ37" s="16"/>
       <c r="DK37" s="16"/>
-      <c r="DL37" s="59" t="s">
-        <v>54</v>
-      </c>
+      <c r="DL37" s="16"/>
       <c r="DM37" s="16"/>
       <c r="DN37" s="16"/>
       <c r="DO37" s="14"/>
@@ -25767,7 +25768,7 @@
       <c r="HK37" s="16"/>
       <c r="HL37" s="16"/>
       <c r="HM37" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="HN37" s="16"/>
       <c r="HO37" s="16"/>
@@ -26016,7 +26017,9 @@
       <c r="CT38" s="14"/>
       <c r="CU38" s="14"/>
       <c r="CV38" s="23"/>
-      <c r="CW38" s="16"/>
+      <c r="CW38" s="90" t="s">
+        <v>53</v>
+      </c>
       <c r="CX38" s="23"/>
       <c r="CY38" s="16"/>
       <c r="CZ38" s="16"/>
@@ -26031,9 +26034,7 @@
       <c r="DI38" s="14"/>
       <c r="DJ38" s="23"/>
       <c r="DK38" s="16"/>
-      <c r="DL38" s="122" t="s">
-        <v>53</v>
-      </c>
+      <c r="DL38" s="16"/>
       <c r="DM38" s="16"/>
       <c r="DN38" s="16"/>
       <c r="DO38" s="14"/>
@@ -26450,7 +26451,7 @@
       <c r="FD39" s="71"/>
       <c r="FE39" s="72"/>
       <c r="FF39" s="158" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="FG39" s="71"/>
       <c r="FH39" s="71"/>
@@ -26759,10 +26760,10 @@
       <c r="CQ40" s="76"/>
       <c r="CR40" s="76"/>
       <c r="CS40" s="76"/>
-      <c r="CT40" s="77" t="s">
-        <v>71</v>
-      </c>
-      <c r="CU40" s="77"/>
+      <c r="CT40" s="80" t="s">
+        <v>111</v>
+      </c>
+      <c r="CU40" s="80"/>
       <c r="CV40" s="78"/>
       <c r="CW40" s="76"/>
       <c r="CX40" s="76"/>
@@ -27176,7 +27177,7 @@
       <c r="EF41" s="16"/>
       <c r="EG41" s="16"/>
       <c r="EH41" s="59" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="EI41" s="59"/>
       <c r="EJ41" s="59"/>
@@ -27569,7 +27570,7 @@
       <c r="FA42" s="16"/>
       <c r="FB42" s="14"/>
       <c r="FC42" s="59" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="FD42" s="59"/>
       <c r="FE42" s="59"/>
@@ -28622,7 +28623,7 @@
       <c r="CR45" s="76"/>
       <c r="CS45" s="76"/>
       <c r="CT45" s="77" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="CU45" s="77"/>
       <c r="CV45" s="46"/>
@@ -30212,7 +30213,7 @@
       <c r="GN49" s="72"/>
       <c r="GO49" s="72"/>
       <c r="GP49" s="144" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="GQ49" s="71"/>
       <c r="GR49" s="144"/>
@@ -30307,7 +30308,7 @@
       <c r="KA49" s="72"/>
       <c r="KB49" s="72"/>
       <c r="KC49" s="144" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="KD49" s="71"/>
       <c r="KE49" s="71"/>
@@ -30492,7 +30493,7 @@
       <c r="CR50" s="76"/>
       <c r="CS50" s="76"/>
       <c r="CT50" s="77" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="CU50" s="77"/>
       <c r="CV50" s="78"/>
@@ -30656,7 +30657,7 @@
       <c r="IT50" s="76"/>
       <c r="IU50" s="76"/>
       <c r="IV50" s="88" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="IW50" s="88"/>
       <c r="IX50" s="88"/>
@@ -30960,7 +30961,7 @@
       <c r="GF51" s="16"/>
       <c r="GG51" s="14"/>
       <c r="GH51" s="59" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="GI51" s="59"/>
       <c r="GJ51" s="59"/>
@@ -31005,7 +31006,7 @@
       <c r="HW51" s="14"/>
       <c r="HX51" s="14"/>
       <c r="HY51" s="59" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="HZ51" s="59"/>
       <c r="IA51" s="59"/>
@@ -31037,7 +31038,7 @@
       <c r="JA51" s="16"/>
       <c r="JB51" s="16"/>
       <c r="JC51" s="59" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="JD51" s="59"/>
       <c r="JE51" s="59"/>
@@ -31058,7 +31059,7 @@
       <c r="JT51" s="59"/>
       <c r="JU51" s="59"/>
       <c r="JV51" s="59" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="JW51" s="59"/>
       <c r="JX51" s="59"/>
@@ -31067,7 +31068,7 @@
       <c r="KA51" s="59"/>
       <c r="KB51" s="59"/>
       <c r="KC51" s="59" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="KD51" s="59"/>
       <c r="KE51" s="59"/>
@@ -31403,7 +31404,7 @@
       <c r="IQ52" s="16"/>
       <c r="IR52" s="14"/>
       <c r="IS52" s="59" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="IT52" s="59"/>
       <c r="IU52" s="59"/>
@@ -32276,11 +32277,6 @@
     <row r="71" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="GA6:HE6"/>
-    <mergeCell ref="HF6:IJ6"/>
-    <mergeCell ref="IK6:JN6"/>
-    <mergeCell ref="JO6:KS6"/>
-    <mergeCell ref="KT6:LW6"/>
     <mergeCell ref="LX6:NB6"/>
     <mergeCell ref="A50:A54"/>
     <mergeCell ref="A15:A19"/>
@@ -32297,6 +32293,11 @@
     <mergeCell ref="BI6:CM6"/>
     <mergeCell ref="CN6:DQ6"/>
     <mergeCell ref="DR6:EV6"/>
+    <mergeCell ref="GA6:HE6"/>
+    <mergeCell ref="HF6:IJ6"/>
+    <mergeCell ref="IK6:JN6"/>
+    <mergeCell ref="JO6:KS6"/>
+    <mergeCell ref="KT6:LW6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[DOC] LF GEN Main 일정 조정
</commit_message>
<xml_diff>
--- a/0_DOC/Femto Project schedule V1.0.xlsx
+++ b/0_DOC/Femto Project schedule V1.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="20180207" sheetId="18" r:id="rId1"/>
@@ -281,7 +281,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="124">
   <si>
     <t>◇PCB설계</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -756,10 +756,6 @@
   </si>
   <si>
     <t>◇부품입고</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>◇PCB설계</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -6847,16 +6843,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>127</xdr:col>
+      <xdr:col>125</xdr:col>
       <xdr:colOff>115544</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>94059</xdr:rowOff>
+      <xdr:rowOff>82853</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>131</xdr:col>
-      <xdr:colOff>171452</xdr:colOff>
+      <xdr:colOff>156883</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>94059</xdr:rowOff>
+      <xdr:rowOff>82853</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -6865,8 +6861,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8407897" y="3343765"/>
-          <a:ext cx="862731" cy="0"/>
+          <a:off x="8004485" y="3332559"/>
+          <a:ext cx="1251574" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -7314,13 +7310,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>127</xdr:col>
+      <xdr:col>138</xdr:col>
       <xdr:colOff>112182</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>87897</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>131</xdr:col>
+      <xdr:col>142</xdr:col>
       <xdr:colOff>168089</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>87897</xdr:rowOff>
@@ -7365,14 +7361,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>119</xdr:col>
-      <xdr:colOff>197907</xdr:colOff>
+      <xdr:col>126</xdr:col>
+      <xdr:colOff>186701</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>86216</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>126</xdr:col>
-      <xdr:colOff>156883</xdr:colOff>
+      <xdr:col>133</xdr:col>
+      <xdr:colOff>145677</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>86216</xdr:rowOff>
     </xdr:to>
@@ -7383,7 +7379,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6876613" y="6552010"/>
+          <a:off x="8277348" y="6552010"/>
           <a:ext cx="1370917" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -7877,14 +7873,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>124</xdr:col>
-      <xdr:colOff>106019</xdr:colOff>
+      <xdr:col>125</xdr:col>
+      <xdr:colOff>94813</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>103585</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>128</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
+      <xdr:col>129</xdr:col>
+      <xdr:colOff>150719</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>103585</xdr:rowOff>
     </xdr:to>
@@ -7895,8 +7891,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="25737794" y="3408760"/>
-          <a:ext cx="856006" cy="0"/>
+          <a:off x="7983754" y="4216144"/>
+          <a:ext cx="862730" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -35037,6 +35033,11 @@
     <row r="71" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="GA6:HE6"/>
+    <mergeCell ref="HF6:IJ6"/>
+    <mergeCell ref="IK6:JN6"/>
+    <mergeCell ref="JO6:KS6"/>
+    <mergeCell ref="KT6:LW6"/>
     <mergeCell ref="LX6:NB6"/>
     <mergeCell ref="A50:A54"/>
     <mergeCell ref="A15:A19"/>
@@ -35053,11 +35054,6 @@
     <mergeCell ref="BI6:CM6"/>
     <mergeCell ref="CN6:DQ6"/>
     <mergeCell ref="DR6:EV6"/>
-    <mergeCell ref="GA6:HE6"/>
-    <mergeCell ref="HF6:IJ6"/>
-    <mergeCell ref="IK6:JN6"/>
-    <mergeCell ref="JO6:KS6"/>
-    <mergeCell ref="KT6:LW6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35071,9 +35067,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:NB71"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="FJ32" sqref="FJ32"/>
+      <selection pane="topRight" activeCell="DX46" sqref="DX46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -36730,7 +36726,7 @@
       <c r="DH8" s="38"/>
       <c r="DI8" s="38"/>
       <c r="DJ8" s="49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="DK8" s="35"/>
       <c r="DL8" s="36"/>
@@ -37502,7 +37498,7 @@
       <c r="DL10" s="30"/>
       <c r="DM10" s="30"/>
       <c r="DN10" s="30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="DO10" s="31"/>
       <c r="DP10" s="31"/>
@@ -39768,7 +39764,7 @@
       <c r="EN16" s="16"/>
       <c r="EO16" s="16"/>
       <c r="EP16" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="EQ16" s="14"/>
       <c r="ER16" s="14"/>
@@ -40113,7 +40109,7 @@
       <c r="DO17" s="14"/>
       <c r="DP17" s="14"/>
       <c r="DQ17" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="DR17" s="67"/>
       <c r="DS17" s="16"/>
@@ -41224,15 +41220,15 @@
       <c r="DJ20" s="76"/>
       <c r="DK20" s="43"/>
       <c r="DL20" s="76"/>
-      <c r="DM20" s="76"/>
-      <c r="DN20" s="76"/>
-      <c r="DO20" s="123" t="s">
+      <c r="DM20" s="123" t="s">
         <v>9</v>
       </c>
+      <c r="DN20" s="60"/>
+      <c r="DO20" s="60"/>
       <c r="DP20" s="60"/>
       <c r="DQ20" s="60"/>
-      <c r="DR20" s="60"/>
-      <c r="DS20" s="60"/>
+      <c r="DR20" s="82"/>
+      <c r="DS20" s="76"/>
       <c r="DT20" s="76"/>
       <c r="DU20" s="76"/>
       <c r="DV20" s="77"/>
@@ -41245,7 +41241,7 @@
       <c r="EC20" s="77"/>
       <c r="ED20" s="77"/>
       <c r="EE20" s="60" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="EF20" s="60"/>
       <c r="EG20" s="60"/>
@@ -41606,15 +41602,15 @@
       <c r="DJ21" s="13"/>
       <c r="DK21" s="16"/>
       <c r="DL21" s="16"/>
-      <c r="DM21" s="16"/>
-      <c r="DN21" s="16"/>
-      <c r="DO21" s="59" t="s">
+      <c r="DM21" s="59" t="s">
         <v>0</v>
       </c>
+      <c r="DN21" s="59"/>
+      <c r="DO21" s="59"/>
       <c r="DP21" s="59"/>
       <c r="DQ21" s="59"/>
-      <c r="DR21" s="59"/>
-      <c r="DS21" s="59"/>
+      <c r="DR21" s="67"/>
+      <c r="DS21" s="16"/>
       <c r="DT21" s="16"/>
       <c r="DU21" s="16"/>
       <c r="DV21" s="14"/>
@@ -42358,11 +42354,11 @@
       <c r="DO23" s="14"/>
       <c r="DP23" s="14"/>
       <c r="DQ23" s="17"/>
-      <c r="DR23" s="67"/>
+      <c r="DR23" s="122" t="s">
+        <v>53</v>
+      </c>
       <c r="DS23" s="16"/>
-      <c r="DT23" s="122" t="s">
-        <v>53</v>
-      </c>
+      <c r="DT23" s="16"/>
       <c r="DU23" s="16"/>
       <c r="DV23" s="14"/>
       <c r="DW23" s="14"/>
@@ -42734,9 +42730,9 @@
       <c r="DO24" s="20"/>
       <c r="DP24" s="20"/>
       <c r="DQ24" s="22"/>
-      <c r="DR24" s="70"/>
-      <c r="DS24" s="71"/>
-      <c r="DT24" s="71"/>
+      <c r="DR24" s="68"/>
+      <c r="DS24" s="21"/>
+      <c r="DT24" s="21"/>
       <c r="DU24" s="71"/>
       <c r="DV24" s="72"/>
       <c r="DW24" s="72"/>
@@ -43112,8 +43108,10 @@
       <c r="DM25" s="76"/>
       <c r="DN25" s="76"/>
       <c r="DO25" s="77"/>
-      <c r="DP25" s="77"/>
-      <c r="DQ25" s="84"/>
+      <c r="DP25" s="145" t="s">
+        <v>9</v>
+      </c>
+      <c r="DQ25" s="88"/>
       <c r="DR25" s="82"/>
       <c r="DS25" s="76"/>
       <c r="DT25" s="76"/>
@@ -43486,8 +43484,10 @@
       <c r="DM26" s="16"/>
       <c r="DN26" s="16"/>
       <c r="DO26" s="14"/>
-      <c r="DP26" s="14"/>
-      <c r="DQ26" s="25"/>
+      <c r="DP26" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="DQ26" s="59"/>
       <c r="DR26" s="67"/>
       <c r="DS26" s="16"/>
       <c r="DT26" s="16"/>
@@ -44231,10 +44231,10 @@
       <c r="DN28" s="13"/>
       <c r="DO28" s="14"/>
       <c r="DP28" s="14"/>
-      <c r="DQ28" s="122" t="s">
+      <c r="DQ28" s="155"/>
+      <c r="DR28" s="122" t="s">
         <v>53</v>
       </c>
-      <c r="DR28" s="13"/>
       <c r="DS28" s="13"/>
       <c r="DT28" s="13"/>
       <c r="DU28" s="13"/>
@@ -44242,14 +44242,14 @@
       <c r="DW28" s="14"/>
       <c r="DX28" s="14"/>
       <c r="DY28" s="13"/>
-      <c r="DZ28" s="59" t="s">
+      <c r="DZ28" s="16"/>
+      <c r="EA28" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="EA28" s="59"/>
       <c r="EB28" s="59"/>
       <c r="EC28" s="59"/>
       <c r="ED28" s="59"/>
-      <c r="EE28" s="13"/>
+      <c r="EE28" s="59"/>
       <c r="EF28" s="16"/>
       <c r="EG28" s="16"/>
       <c r="EH28" s="16"/>
@@ -47980,7 +47980,9 @@
       <c r="EE38" s="13"/>
       <c r="EF38" s="16"/>
       <c r="EG38" s="16"/>
-      <c r="EH38" s="16"/>
+      <c r="EH38" s="16" t="s">
+        <v>73</v>
+      </c>
       <c r="EI38" s="16"/>
       <c r="EJ38" s="14"/>
       <c r="EK38" s="14"/>
@@ -48703,11 +48705,11 @@
       <c r="DF40" s="80"/>
       <c r="DG40" s="80"/>
       <c r="DH40" s="80"/>
-      <c r="DI40" s="88"/>
-      <c r="DJ40" s="88"/>
-      <c r="DK40" s="88"/>
-      <c r="DL40" s="88"/>
-      <c r="DM40" s="88"/>
+      <c r="DI40" s="80"/>
+      <c r="DJ40" s="80"/>
+      <c r="DK40" s="80"/>
+      <c r="DL40" s="80"/>
+      <c r="DM40" s="76"/>
       <c r="DN40" s="76"/>
       <c r="DO40" s="77"/>
       <c r="DP40" s="77"/>
@@ -49080,23 +49082,23 @@
       <c r="DI41" s="14"/>
       <c r="DJ41" s="13"/>
       <c r="DK41" s="16"/>
-      <c r="DL41" s="59" t="s">
-        <v>119</v>
-      </c>
-      <c r="DM41" s="59"/>
-      <c r="DN41" s="59"/>
-      <c r="DO41" s="59"/>
-      <c r="DP41" s="59"/>
-      <c r="DQ41" s="161"/>
-      <c r="DR41" s="101"/>
-      <c r="DS41" s="59"/>
-      <c r="DT41" s="16"/>
-      <c r="DU41" s="16"/>
-      <c r="DV41" s="14"/>
-      <c r="DW41" s="14"/>
-      <c r="DX41" s="14"/>
-      <c r="DY41" s="16"/>
-      <c r="DZ41" s="16"/>
+      <c r="DL41" s="16"/>
+      <c r="DM41" s="16"/>
+      <c r="DN41" s="16"/>
+      <c r="DO41" s="14"/>
+      <c r="DP41" s="14"/>
+      <c r="DQ41" s="25"/>
+      <c r="DR41" s="67"/>
+      <c r="DS41" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="DT41" s="59"/>
+      <c r="DU41" s="59"/>
+      <c r="DV41" s="59"/>
+      <c r="DW41" s="59"/>
+      <c r="DX41" s="59"/>
+      <c r="DY41" s="59"/>
+      <c r="DZ41" s="59"/>
       <c r="EA41" s="16"/>
       <c r="EB41" s="16"/>
       <c r="EC41" s="14"/>
@@ -49450,16 +49452,16 @@
       <c r="DI42" s="14"/>
       <c r="DJ42" s="13"/>
       <c r="DK42" s="16"/>
-      <c r="DL42" s="59" t="s">
-        <v>54</v>
-      </c>
+      <c r="DL42" s="16"/>
       <c r="DM42" s="16"/>
       <c r="DN42" s="16"/>
       <c r="DO42" s="14"/>
       <c r="DP42" s="14"/>
       <c r="DQ42" s="25"/>
       <c r="DR42" s="67"/>
-      <c r="DS42" s="16"/>
+      <c r="DS42" s="59" t="s">
+        <v>54</v>
+      </c>
       <c r="DT42" s="16"/>
       <c r="DU42" s="16"/>
       <c r="DV42" s="14"/>
@@ -49828,10 +49830,6 @@
       <c r="DQ43" s="17"/>
       <c r="DR43" s="67"/>
       <c r="DS43" s="16"/>
-      <c r="DT43" s="122" t="s">
-        <v>53</v>
-      </c>
-      <c r="DU43" s="16"/>
       <c r="DV43" s="14"/>
       <c r="DW43" s="14"/>
       <c r="DX43" s="14"/>
@@ -49841,11 +49839,11 @@
       <c r="EB43" s="16"/>
       <c r="EC43" s="14"/>
       <c r="ED43" s="14"/>
-      <c r="EE43" s="59" t="s">
-        <v>39</v>
-      </c>
-      <c r="EF43" s="59"/>
-      <c r="EG43" s="59"/>
+      <c r="EE43" s="122" t="s">
+        <v>53</v>
+      </c>
+      <c r="EF43" s="16"/>
+      <c r="EG43" s="16"/>
       <c r="EH43" s="16"/>
       <c r="EI43" s="16"/>
       <c r="EJ43" s="14"/>
@@ -49854,9 +49852,11 @@
       <c r="EM43" s="14"/>
       <c r="EN43" s="16"/>
       <c r="EO43" s="16"/>
-      <c r="EP43" s="16"/>
-      <c r="EQ43" s="14"/>
-      <c r="ER43" s="14"/>
+      <c r="EP43" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="EQ43" s="59"/>
+      <c r="ER43" s="59"/>
       <c r="ES43" s="13"/>
       <c r="ET43" s="13"/>
       <c r="EU43" s="13"/>
@@ -54203,15 +54203,6 @@
     <row r="71" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="A45:A49"/>
-    <mergeCell ref="A50:A54"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A30:A34"/>
-    <mergeCell ref="A35:A39"/>
     <mergeCell ref="LX6:NB6"/>
     <mergeCell ref="B6:AF6"/>
     <mergeCell ref="AG6:BH6"/>
@@ -54224,6 +54215,15 @@
     <mergeCell ref="IK6:JN6"/>
     <mergeCell ref="JO6:KS6"/>
     <mergeCell ref="KT6:LW6"/>
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="A35:A39"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>